<commit_message>
Started the SQUID and am working on calculating nutrient averages to add to LIMs
</commit_message>
<xml_diff>
--- a/environmental_data/for_humans/Copy of GEODES_TNTP.xlsx
+++ b/environmental_data/for_humans/Copy of GEODES_TNTP.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17927"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,19 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1070" uniqueCount="204">
   <si>
     <t>F/SP_7-6_5AM1</t>
   </si>
@@ -522,12 +522,123 @@
   </si>
   <si>
     <t>Unfiltered</t>
+  </si>
+  <si>
+    <t>Sample</t>
+  </si>
+  <si>
+    <t>TDN</t>
+  </si>
+  <si>
+    <t>TDP</t>
+  </si>
+  <si>
+    <t>GEODES_ME_0hr</t>
+  </si>
+  <si>
+    <t>GEODES_ME_12hr</t>
+  </si>
+  <si>
+    <t>GEODES_ME_16hr</t>
+  </si>
+  <si>
+    <t>GEODES_ME_20hr</t>
+  </si>
+  <si>
+    <t>GEODES_ME_24hr</t>
+  </si>
+  <si>
+    <t>GEODES_ME_28hr</t>
+  </si>
+  <si>
+    <t>GEODES_ME_32hr</t>
+  </si>
+  <si>
+    <t>GEODES_ME_36hr</t>
+  </si>
+  <si>
+    <t>GEODES_ME_4hr</t>
+  </si>
+  <si>
+    <t>GEODES_ME_8hr</t>
+  </si>
+  <si>
+    <t>GEODES_SP_0hr</t>
+  </si>
+  <si>
+    <t>GEODES_SP_12hr</t>
+  </si>
+  <si>
+    <t>GEODES_SP_16hr</t>
+  </si>
+  <si>
+    <t>GEODES_SP_20hr</t>
+  </si>
+  <si>
+    <t>GEODES_SP_24hr</t>
+  </si>
+  <si>
+    <t>GEODES_SP_28hr</t>
+  </si>
+  <si>
+    <t>GEODES_SP_32hr</t>
+  </si>
+  <si>
+    <t>GEODES_SP_36hr</t>
+  </si>
+  <si>
+    <t>GEODES_SP_4hr</t>
+  </si>
+  <si>
+    <t>GEODES_SP_8hr</t>
+  </si>
+  <si>
+    <t>GEODES_SP_40hr</t>
+  </si>
+  <si>
+    <t>GEODES_TB_0hr</t>
+  </si>
+  <si>
+    <t>GEODES_TB_12hr</t>
+  </si>
+  <si>
+    <t>GEODES_TB_16hr</t>
+  </si>
+  <si>
+    <t>GEODES_TB_24hr</t>
+  </si>
+  <si>
+    <t>GEODES_TB_28hr</t>
+  </si>
+  <si>
+    <t>GEODES_TB_32hr</t>
+  </si>
+  <si>
+    <t>GEODES_TB_36hr</t>
+  </si>
+  <si>
+    <t>GEODES_TB_40hr</t>
+  </si>
+  <si>
+    <t>GEODES_TB_4hr</t>
+  </si>
+  <si>
+    <t>GEODES_TB_8hr</t>
+  </si>
+  <si>
+    <t>GEODES_TB_44hr</t>
+  </si>
+  <si>
+    <t>TN/TDN and TP/TDP are the averages of 2 replicates each.</t>
+  </si>
+  <si>
+    <t>Cyanotoxins measured by Todd Miller's lab.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
@@ -560,11 +671,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -902,11 +1014,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G145"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4266,7 +4378,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E191"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5885,13 +5997,3622 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:U145"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U2" sqref="U2:U3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="6" max="6" width="4.28515625" customWidth="1"/>
+    <col min="7" max="10" width="9.140625" style="4"/>
+    <col min="11" max="13" width="2.7109375" customWidth="1"/>
+    <col min="14" max="14" width="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7.7109375" style="4" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D1" t="s">
+        <v>168</v>
+      </c>
+      <c r="E1" t="s">
+        <v>169</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="N1" t="s">
+        <v>149</v>
+      </c>
+      <c r="O1" t="s">
+        <v>153</v>
+      </c>
+      <c r="P1" t="s">
+        <v>150</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>165</v>
+      </c>
+      <c r="R1" t="s">
+        <v>158</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>170</v>
+      </c>
+      <c r="G2" s="4">
+        <f>AVERAGE(T4:T5)</f>
+        <v>616.59699999999998</v>
+      </c>
+      <c r="H2" s="4">
+        <f>AVERAGE(S4:S5)</f>
+        <v>18.738999999999997</v>
+      </c>
+      <c r="I2" s="4">
+        <f>AVERAGE(T2:T3)</f>
+        <v>500.24849999999998</v>
+      </c>
+      <c r="J2" s="4">
+        <f>AVERAGE(S2:S3)</f>
+        <v>7.8554999999999993</v>
+      </c>
+      <c r="N2" t="s">
+        <v>156</v>
+      </c>
+      <c r="O2" s="2">
+        <v>42565</v>
+      </c>
+      <c r="P2" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q2">
+        <v>1</v>
+      </c>
+      <c r="R2" t="s">
+        <v>157</v>
+      </c>
+      <c r="S2" s="4">
+        <v>8.0139999999999993</v>
+      </c>
+      <c r="T2" s="4">
+        <v>518.15499999999997</v>
+      </c>
+      <c r="U2" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>171</v>
+      </c>
+      <c r="G3" s="4">
+        <f>AVERAGE(T16:T17)</f>
+        <v>713.89850000000001</v>
+      </c>
+      <c r="H3" s="4">
+        <f>AVERAGE(S16:S17)</f>
+        <v>19.43</v>
+      </c>
+      <c r="I3" s="4">
+        <f>AVERAGE(T14:T15)</f>
+        <v>509.00850000000003</v>
+      </c>
+      <c r="J3" s="4">
+        <f>AVERAGE(S14:S15)</f>
+        <v>9.2100000000000009</v>
+      </c>
+      <c r="N3" t="s">
+        <v>156</v>
+      </c>
+      <c r="O3" s="2">
+        <v>42565</v>
+      </c>
+      <c r="P3" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q3">
+        <v>2</v>
+      </c>
+      <c r="R3" t="s">
+        <v>157</v>
+      </c>
+      <c r="S3" s="4">
+        <v>7.6970000000000001</v>
+      </c>
+      <c r="T3" s="4">
+        <v>482.34199999999998</v>
+      </c>
+      <c r="U3" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>172</v>
+      </c>
+      <c r="G4" s="4">
+        <f>AVERAGE(T20:T21)</f>
+        <v>618.98299999999995</v>
+      </c>
+      <c r="H4" s="4">
+        <f>AVERAGE(S20:S21)</f>
+        <v>18.357500000000002</v>
+      </c>
+      <c r="I4" s="4">
+        <f>AVERAGE(T18:T19)</f>
+        <v>507.726</v>
+      </c>
+      <c r="J4" s="4">
+        <f>AVERAGE(S18:S19)</f>
+        <v>9.7949999999999999</v>
+      </c>
+      <c r="N4" t="s">
+        <v>156</v>
+      </c>
+      <c r="O4" s="2">
+        <v>42565</v>
+      </c>
+      <c r="P4" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q4">
+        <v>1</v>
+      </c>
+      <c r="R4" t="s">
+        <v>166</v>
+      </c>
+      <c r="S4" s="4">
+        <v>18.835999999999999</v>
+      </c>
+      <c r="T4" s="4">
+        <v>591.36699999999996</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>173</v>
+      </c>
+      <c r="G5" s="4">
+        <f>AVERAGE(T24:T25)</f>
+        <v>662.30449999999996</v>
+      </c>
+      <c r="H5" s="4">
+        <f>AVERAGE(S24:S25)</f>
+        <v>22.120999999999999</v>
+      </c>
+      <c r="I5" s="4">
+        <f>AVERAGE(T22:T23)</f>
+        <v>508.37599999999998</v>
+      </c>
+      <c r="J5" s="4">
+        <f>AVERAGE(S22:S23)</f>
+        <v>8.7585000000000015</v>
+      </c>
+      <c r="N5" t="s">
+        <v>156</v>
+      </c>
+      <c r="O5" s="2">
+        <v>42565</v>
+      </c>
+      <c r="P5" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q5">
+        <v>2</v>
+      </c>
+      <c r="R5" t="s">
+        <v>166</v>
+      </c>
+      <c r="S5" s="4">
+        <v>18.641999999999999</v>
+      </c>
+      <c r="T5" s="4">
+        <v>641.827</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>174</v>
+      </c>
+      <c r="G6" s="4">
+        <f>AVERAGE(T28:T29)</f>
+        <v>592.33749999999998</v>
+      </c>
+      <c r="H6" s="4">
+        <f>AVERAGE(S28:S29)</f>
+        <v>18.023499999999999</v>
+      </c>
+      <c r="I6" s="4">
+        <f>AVERAGE(T26:T27)</f>
+        <v>470.13</v>
+      </c>
+      <c r="J6" s="4">
+        <f>AVERAGE(S26:S27)</f>
+        <v>7.0404999999999998</v>
+      </c>
+      <c r="N6" t="s">
+        <v>156</v>
+      </c>
+      <c r="O6" s="2">
+        <v>42565</v>
+      </c>
+      <c r="P6" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q6">
+        <v>1</v>
+      </c>
+      <c r="R6" t="s">
+        <v>157</v>
+      </c>
+      <c r="S6" s="4">
+        <v>10.257999999999999</v>
+      </c>
+      <c r="T6" s="4">
+        <v>566.66300000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>175</v>
+      </c>
+      <c r="G7" s="4">
+        <f>AVERAGE(T32:T33)</f>
+        <v>623.79349999999999</v>
+      </c>
+      <c r="H7" s="4">
+        <f>AVERAGE(S32:S33)</f>
+        <v>19.7105</v>
+      </c>
+      <c r="I7" s="4">
+        <f>AVERAGE(T30:T31)</f>
+        <v>507.19499999999999</v>
+      </c>
+      <c r="J7" s="4">
+        <f>AVERAGE(S30:S31)</f>
+        <v>9.4700000000000006</v>
+      </c>
+      <c r="N7" t="s">
+        <v>156</v>
+      </c>
+      <c r="O7" s="2">
+        <v>42565</v>
+      </c>
+      <c r="P7" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q7">
+        <v>2</v>
+      </c>
+      <c r="R7" t="s">
+        <v>157</v>
+      </c>
+      <c r="S7" s="4">
+        <v>10.488</v>
+      </c>
+      <c r="T7" s="4">
+        <v>531.00900000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>176</v>
+      </c>
+      <c r="G8" s="4">
+        <f>AVERAGE(T36:T37)</f>
+        <v>580.84799999999996</v>
+      </c>
+      <c r="H8" s="4">
+        <f>AVERAGE(S36:S37)</f>
+        <v>15.785500000000001</v>
+      </c>
+      <c r="I8" s="4">
+        <f>AVERAGE(T34:T35)</f>
+        <v>517.39499999999998</v>
+      </c>
+      <c r="J8" s="4">
+        <f>AVERAGE(S34:S35)</f>
+        <v>8.1509999999999998</v>
+      </c>
+      <c r="N8" t="s">
+        <v>156</v>
+      </c>
+      <c r="O8" s="2">
+        <v>42565</v>
+      </c>
+      <c r="P8" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q8">
+        <v>1</v>
+      </c>
+      <c r="R8" t="s">
+        <v>166</v>
+      </c>
+      <c r="S8" s="4">
+        <v>18.885999999999999</v>
+      </c>
+      <c r="T8" s="4">
+        <v>671.48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>177</v>
+      </c>
+      <c r="G9" s="4">
+        <f>AVERAGE(T40:T41)</f>
+        <v>586.37950000000001</v>
+      </c>
+      <c r="H9" s="4">
+        <f>AVERAGE(S40:S41)</f>
+        <v>17.075500000000002</v>
+      </c>
+      <c r="I9" s="4">
+        <f>AVERAGE(T38:T39)</f>
+        <v>500.005</v>
+      </c>
+      <c r="J9" s="4">
+        <f>AVERAGE(S38:S39)</f>
+        <v>8.7684999999999995</v>
+      </c>
+      <c r="N9" t="s">
+        <v>156</v>
+      </c>
+      <c r="O9" s="2">
+        <v>42565</v>
+      </c>
+      <c r="P9" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q9">
+        <v>2</v>
+      </c>
+      <c r="R9" t="s">
+        <v>166</v>
+      </c>
+      <c r="S9" s="4">
+        <v>20.881</v>
+      </c>
+      <c r="T9" s="4">
+        <v>658.71600000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>178</v>
+      </c>
+      <c r="N10" t="s">
+        <v>156</v>
+      </c>
+      <c r="O10" s="2">
+        <v>42565</v>
+      </c>
+      <c r="P10" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q10">
+        <v>1</v>
+      </c>
+      <c r="R10" t="s">
+        <v>157</v>
+      </c>
+      <c r="S10" s="4">
+        <v>8.4969999999999999</v>
+      </c>
+      <c r="T10" s="4">
+        <v>513.42399999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>179</v>
+      </c>
+      <c r="N11" t="s">
+        <v>156</v>
+      </c>
+      <c r="O11" s="2">
+        <v>42565</v>
+      </c>
+      <c r="P11" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q11">
+        <v>2</v>
+      </c>
+      <c r="R11" t="s">
+        <v>157</v>
+      </c>
+      <c r="S11" s="4">
+        <v>9.2780000000000005</v>
+      </c>
+      <c r="T11" s="4">
+        <v>482.673</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>180</v>
+      </c>
+      <c r="N12" t="s">
+        <v>156</v>
+      </c>
+      <c r="O12" s="2">
+        <v>42565</v>
+      </c>
+      <c r="P12" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q12">
+        <v>1</v>
+      </c>
+      <c r="R12" t="s">
+        <v>166</v>
+      </c>
+      <c r="S12" s="4">
+        <v>17.805</v>
+      </c>
+      <c r="T12" s="4">
+        <v>578.44200000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>181</v>
+      </c>
+      <c r="N13" t="s">
+        <v>156</v>
+      </c>
+      <c r="O13" s="2">
+        <v>42565</v>
+      </c>
+      <c r="P13" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q13">
+        <v>2</v>
+      </c>
+      <c r="R13" t="s">
+        <v>166</v>
+      </c>
+      <c r="S13" s="4">
+        <v>20.215</v>
+      </c>
+      <c r="T13" s="4">
+        <v>617.74800000000005</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>182</v>
+      </c>
+      <c r="N14" t="s">
+        <v>156</v>
+      </c>
+      <c r="O14" s="2">
+        <v>42565</v>
+      </c>
+      <c r="P14" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q14">
+        <v>1</v>
+      </c>
+      <c r="R14" t="s">
+        <v>157</v>
+      </c>
+      <c r="S14" s="4">
+        <v>9.7309999999999999</v>
+      </c>
+      <c r="T14" s="4">
+        <v>512.10400000000004</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>183</v>
+      </c>
+      <c r="N15" t="s">
+        <v>156</v>
+      </c>
+      <c r="O15" s="2">
+        <v>42565</v>
+      </c>
+      <c r="P15" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q15">
+        <v>2</v>
+      </c>
+      <c r="R15" t="s">
+        <v>157</v>
+      </c>
+      <c r="S15" s="4">
+        <v>8.6890000000000001</v>
+      </c>
+      <c r="T15" s="4">
+        <v>505.91300000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>184</v>
+      </c>
+      <c r="N16" t="s">
+        <v>156</v>
+      </c>
+      <c r="O16" s="2">
+        <v>42565</v>
+      </c>
+      <c r="P16" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q16">
+        <v>1</v>
+      </c>
+      <c r="R16" t="s">
+        <v>166</v>
+      </c>
+      <c r="S16" s="4">
+        <v>18.341000000000001</v>
+      </c>
+      <c r="T16" s="4">
+        <v>665.55799999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>185</v>
+      </c>
+      <c r="N17" t="s">
+        <v>156</v>
+      </c>
+      <c r="O17" s="2">
+        <v>42565</v>
+      </c>
+      <c r="P17" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q17">
+        <v>2</v>
+      </c>
+      <c r="R17" t="s">
+        <v>166</v>
+      </c>
+      <c r="S17" s="4">
+        <v>20.518999999999998</v>
+      </c>
+      <c r="T17" s="4">
+        <v>762.23900000000003</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>186</v>
+      </c>
+      <c r="N18" t="s">
+        <v>156</v>
+      </c>
+      <c r="O18" s="2">
+        <v>42565</v>
+      </c>
+      <c r="P18" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q18">
+        <v>1</v>
+      </c>
+      <c r="R18" t="s">
+        <v>157</v>
+      </c>
+      <c r="S18" s="4">
+        <v>9.9559999999999995</v>
+      </c>
+      <c r="T18" s="4">
+        <v>520.96299999999997</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>187</v>
+      </c>
+      <c r="N19" t="s">
+        <v>156</v>
+      </c>
+      <c r="O19" s="2">
+        <v>42565</v>
+      </c>
+      <c r="P19" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q19">
+        <v>2</v>
+      </c>
+      <c r="R19" t="s">
+        <v>157</v>
+      </c>
+      <c r="S19" s="4">
+        <v>9.6340000000000003</v>
+      </c>
+      <c r="T19" s="4">
+        <v>494.48899999999998</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>190</v>
+      </c>
+      <c r="N20" t="s">
+        <v>156</v>
+      </c>
+      <c r="O20" s="2">
+        <v>42565</v>
+      </c>
+      <c r="P20" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q20">
+        <v>1</v>
+      </c>
+      <c r="R20" t="s">
+        <v>166</v>
+      </c>
+      <c r="S20" s="4">
+        <v>17.975999999999999</v>
+      </c>
+      <c r="T20" s="4">
+        <v>617.21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>188</v>
+      </c>
+      <c r="N21" t="s">
+        <v>156</v>
+      </c>
+      <c r="O21" s="2">
+        <v>42565</v>
+      </c>
+      <c r="P21" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q21">
+        <v>2</v>
+      </c>
+      <c r="R21" t="s">
+        <v>166</v>
+      </c>
+      <c r="S21" s="4">
+        <v>18.739000000000001</v>
+      </c>
+      <c r="T21" s="4">
+        <v>620.75599999999997</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>189</v>
+      </c>
+      <c r="N22" t="s">
+        <v>156</v>
+      </c>
+      <c r="O22" s="2">
+        <v>42566</v>
+      </c>
+      <c r="P22" t="s">
+        <v>164</v>
+      </c>
+      <c r="Q22">
+        <v>1</v>
+      </c>
+      <c r="R22" t="s">
+        <v>157</v>
+      </c>
+      <c r="S22" s="4">
+        <v>8.6240000000000006</v>
+      </c>
+      <c r="T22" s="4">
+        <v>506.33800000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>191</v>
+      </c>
+      <c r="N23" t="s">
+        <v>156</v>
+      </c>
+      <c r="O23" s="2">
+        <v>42566</v>
+      </c>
+      <c r="P23" t="s">
+        <v>164</v>
+      </c>
+      <c r="Q23">
+        <v>2</v>
+      </c>
+      <c r="R23" t="s">
+        <v>157</v>
+      </c>
+      <c r="S23" s="4">
+        <v>8.8930000000000007</v>
+      </c>
+      <c r="T23" s="4">
+        <v>510.41399999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>192</v>
+      </c>
+      <c r="N24" t="s">
+        <v>156</v>
+      </c>
+      <c r="O24" s="2">
+        <v>42566</v>
+      </c>
+      <c r="P24" t="s">
+        <v>164</v>
+      </c>
+      <c r="Q24">
+        <v>1</v>
+      </c>
+      <c r="R24" t="s">
+        <v>166</v>
+      </c>
+      <c r="S24" s="4">
+        <v>21.254999999999999</v>
+      </c>
+      <c r="T24" s="4">
+        <v>672.173</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>193</v>
+      </c>
+      <c r="N25" t="s">
+        <v>156</v>
+      </c>
+      <c r="O25" s="2">
+        <v>42566</v>
+      </c>
+      <c r="P25" t="s">
+        <v>164</v>
+      </c>
+      <c r="Q25">
+        <v>2</v>
+      </c>
+      <c r="R25" t="s">
+        <v>166</v>
+      </c>
+      <c r="S25" s="4">
+        <v>22.986999999999998</v>
+      </c>
+      <c r="T25" s="4">
+        <v>652.43600000000004</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>194</v>
+      </c>
+      <c r="N26" t="s">
+        <v>156</v>
+      </c>
+      <c r="O26" s="2">
+        <v>42566</v>
+      </c>
+      <c r="P26" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q26">
+        <v>1</v>
+      </c>
+      <c r="R26" t="s">
+        <v>157</v>
+      </c>
+      <c r="S26" s="4">
+        <v>6.24</v>
+      </c>
+      <c r="T26" s="4">
+        <v>470.41399999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>195</v>
+      </c>
+      <c r="N27" t="s">
+        <v>156</v>
+      </c>
+      <c r="O27" s="2">
+        <v>42566</v>
+      </c>
+      <c r="P27" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q27">
+        <v>2</v>
+      </c>
+      <c r="R27" t="s">
+        <v>157</v>
+      </c>
+      <c r="S27" s="4">
+        <v>7.8410000000000002</v>
+      </c>
+      <c r="T27" s="4">
+        <v>469.846</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>196</v>
+      </c>
+      <c r="N28" t="s">
+        <v>156</v>
+      </c>
+      <c r="O28" s="2">
+        <v>42566</v>
+      </c>
+      <c r="P28" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q28">
+        <v>1</v>
+      </c>
+      <c r="R28" t="s">
+        <v>166</v>
+      </c>
+      <c r="S28" s="4">
+        <v>14.407</v>
+      </c>
+      <c r="T28" s="4">
+        <v>572.92999999999995</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>197</v>
+      </c>
+      <c r="N29" t="s">
+        <v>156</v>
+      </c>
+      <c r="O29" s="2">
+        <v>42566</v>
+      </c>
+      <c r="P29" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q29">
+        <v>2</v>
+      </c>
+      <c r="R29" t="s">
+        <v>166</v>
+      </c>
+      <c r="S29" s="4">
+        <v>21.64</v>
+      </c>
+      <c r="T29" s="4">
+        <v>611.745</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>198</v>
+      </c>
+      <c r="N30" t="s">
+        <v>156</v>
+      </c>
+      <c r="O30" s="2">
+        <v>42566</v>
+      </c>
+      <c r="P30" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q30">
+        <v>1</v>
+      </c>
+      <c r="R30" t="s">
+        <v>157</v>
+      </c>
+      <c r="S30" s="4">
+        <v>9.1620000000000008</v>
+      </c>
+      <c r="T30" s="4">
+        <v>502.839</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>201</v>
+      </c>
+      <c r="N31" t="s">
+        <v>156</v>
+      </c>
+      <c r="O31" s="2">
+        <v>42566</v>
+      </c>
+      <c r="P31" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q31">
+        <v>2</v>
+      </c>
+      <c r="R31" t="s">
+        <v>157</v>
+      </c>
+      <c r="S31" s="4">
+        <v>9.7780000000000005</v>
+      </c>
+      <c r="T31" s="4">
+        <v>511.55099999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>199</v>
+      </c>
+      <c r="N32" t="s">
+        <v>156</v>
+      </c>
+      <c r="O32" s="2">
+        <v>42566</v>
+      </c>
+      <c r="P32" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q32">
+        <v>1</v>
+      </c>
+      <c r="R32" t="s">
+        <v>166</v>
+      </c>
+      <c r="S32" s="4">
+        <v>22.827999999999999</v>
+      </c>
+      <c r="T32" s="4">
+        <v>644.05399999999997</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>200</v>
+      </c>
+      <c r="N33" t="s">
+        <v>156</v>
+      </c>
+      <c r="O33" s="2">
+        <v>42566</v>
+      </c>
+      <c r="P33" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q33">
+        <v>2</v>
+      </c>
+      <c r="R33" t="s">
+        <v>166</v>
+      </c>
+      <c r="S33" s="4">
+        <v>16.593</v>
+      </c>
+      <c r="T33" s="4">
+        <v>603.53300000000002</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="N34" t="s">
+        <v>156</v>
+      </c>
+      <c r="O34" s="2">
+        <v>42566</v>
+      </c>
+      <c r="P34" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q34">
+        <v>1</v>
+      </c>
+      <c r="R34" t="s">
+        <v>157</v>
+      </c>
+      <c r="S34" s="4">
+        <v>8.3140000000000001</v>
+      </c>
+      <c r="T34" s="4">
+        <v>504.55900000000003</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="N35" t="s">
+        <v>156</v>
+      </c>
+      <c r="O35" s="2">
+        <v>42566</v>
+      </c>
+      <c r="P35" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q35">
+        <v>2</v>
+      </c>
+      <c r="R35" t="s">
+        <v>157</v>
+      </c>
+      <c r="S35" s="4">
+        <v>7.9880000000000004</v>
+      </c>
+      <c r="T35" s="4">
+        <v>530.23099999999999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="N36" t="s">
+        <v>156</v>
+      </c>
+      <c r="O36" s="2">
+        <v>42566</v>
+      </c>
+      <c r="P36" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q36">
+        <v>1</v>
+      </c>
+      <c r="R36" t="s">
+        <v>166</v>
+      </c>
+      <c r="S36" s="4">
+        <v>16.315000000000001</v>
+      </c>
+      <c r="T36" s="4">
+        <v>591.79999999999995</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="N37" t="s">
+        <v>156</v>
+      </c>
+      <c r="O37" s="2">
+        <v>42566</v>
+      </c>
+      <c r="P37" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q37">
+        <v>2</v>
+      </c>
+      <c r="R37" t="s">
+        <v>166</v>
+      </c>
+      <c r="S37" s="4">
+        <v>15.256</v>
+      </c>
+      <c r="T37" s="4">
+        <v>569.89599999999996</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="N38" t="s">
+        <v>156</v>
+      </c>
+      <c r="O38" s="2">
+        <v>42566</v>
+      </c>
+      <c r="P38" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q38">
+        <v>1</v>
+      </c>
+      <c r="R38" t="s">
+        <v>157</v>
+      </c>
+      <c r="S38" s="4">
+        <v>9.6509999999999998</v>
+      </c>
+      <c r="T38" s="4">
+        <v>507.07600000000002</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="N39" t="s">
+        <v>156</v>
+      </c>
+      <c r="O39" s="2">
+        <v>42566</v>
+      </c>
+      <c r="P39" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q39">
+        <v>2</v>
+      </c>
+      <c r="R39" t="s">
+        <v>157</v>
+      </c>
+      <c r="S39" s="4">
+        <v>7.8860000000000001</v>
+      </c>
+      <c r="T39" s="4">
+        <v>492.93400000000003</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="N40" t="s">
+        <v>156</v>
+      </c>
+      <c r="O40" s="2">
+        <v>42566</v>
+      </c>
+      <c r="P40" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q40">
+        <v>1</v>
+      </c>
+      <c r="R40" t="s">
+        <v>166</v>
+      </c>
+      <c r="S40" s="4">
+        <v>17.042000000000002</v>
+      </c>
+      <c r="T40" s="4">
+        <v>587.56500000000005</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="N41" t="s">
+        <v>156</v>
+      </c>
+      <c r="O41" s="2">
+        <v>42566</v>
+      </c>
+      <c r="P41" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q41">
+        <v>2</v>
+      </c>
+      <c r="R41" t="s">
+        <v>166</v>
+      </c>
+      <c r="S41" s="4">
+        <v>17.109000000000002</v>
+      </c>
+      <c r="T41" s="4">
+        <v>585.19399999999996</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="N42" t="s">
+        <v>156</v>
+      </c>
+      <c r="O42" s="2">
+        <v>42566</v>
+      </c>
+      <c r="P42" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q42">
+        <v>1</v>
+      </c>
+      <c r="R42" t="s">
+        <v>157</v>
+      </c>
+      <c r="S42" s="4">
+        <v>7.7930000000000001</v>
+      </c>
+      <c r="T42" s="4">
+        <v>552.98800000000006</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="N43" t="s">
+        <v>156</v>
+      </c>
+      <c r="O43" s="2">
+        <v>42566</v>
+      </c>
+      <c r="P43" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q43">
+        <v>2</v>
+      </c>
+      <c r="R43" t="s">
+        <v>157</v>
+      </c>
+      <c r="S43" s="4">
+        <v>7.6559999999999997</v>
+      </c>
+      <c r="T43" s="4">
+        <v>688.06299999999999</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="N44" t="s">
+        <v>156</v>
+      </c>
+      <c r="O44" s="2">
+        <v>42566</v>
+      </c>
+      <c r="P44" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q44">
+        <v>1</v>
+      </c>
+      <c r="R44" t="s">
+        <v>166</v>
+      </c>
+      <c r="S44" s="4">
+        <v>16.254000000000001</v>
+      </c>
+      <c r="T44" s="4">
+        <v>628.55600000000004</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="N45" t="s">
+        <v>156</v>
+      </c>
+      <c r="O45" s="2">
+        <v>42566</v>
+      </c>
+      <c r="P45" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q45">
+        <v>2</v>
+      </c>
+      <c r="R45" t="s">
+        <v>166</v>
+      </c>
+      <c r="S45" s="4">
+        <v>16.297999999999998</v>
+      </c>
+      <c r="T45" s="4">
+        <v>629.78599999999994</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="N46" t="s">
+        <v>156</v>
+      </c>
+      <c r="O46" s="2">
+        <v>42567</v>
+      </c>
+      <c r="P46" t="s">
+        <v>164</v>
+      </c>
+      <c r="Q46">
+        <v>1</v>
+      </c>
+      <c r="R46" t="s">
+        <v>157</v>
+      </c>
+      <c r="S46" s="4">
+        <v>7.633</v>
+      </c>
+      <c r="T46" s="4">
+        <v>554.66700000000003</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="N47" t="s">
+        <v>156</v>
+      </c>
+      <c r="O47" s="2">
+        <v>42567</v>
+      </c>
+      <c r="P47" t="s">
+        <v>164</v>
+      </c>
+      <c r="Q47">
+        <v>2</v>
+      </c>
+      <c r="R47" t="s">
+        <v>157</v>
+      </c>
+      <c r="S47" s="4">
+        <v>7.6059999999999999</v>
+      </c>
+      <c r="T47" s="4">
+        <v>568.21400000000006</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="N48" t="s">
+        <v>156</v>
+      </c>
+      <c r="O48" s="2">
+        <v>42567</v>
+      </c>
+      <c r="P48" t="s">
+        <v>164</v>
+      </c>
+      <c r="Q48">
+        <v>1</v>
+      </c>
+      <c r="R48" t="s">
+        <v>166</v>
+      </c>
+      <c r="S48" s="4">
+        <v>18.655999999999999</v>
+      </c>
+      <c r="T48" s="4">
+        <v>677.79</v>
+      </c>
+    </row>
+    <row r="49" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N49" t="s">
+        <v>156</v>
+      </c>
+      <c r="O49" s="2">
+        <v>42567</v>
+      </c>
+      <c r="P49" t="s">
+        <v>164</v>
+      </c>
+      <c r="Q49">
+        <v>2</v>
+      </c>
+      <c r="R49" t="s">
+        <v>166</v>
+      </c>
+      <c r="S49" s="4">
+        <v>17.789000000000001</v>
+      </c>
+      <c r="T49" s="4">
+        <v>659.99900000000002</v>
+      </c>
+    </row>
+    <row r="50" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N50" t="s">
+        <v>154</v>
+      </c>
+      <c r="O50" s="2">
+        <v>42557</v>
+      </c>
+      <c r="P50" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q50">
+        <v>1</v>
+      </c>
+      <c r="R50" t="s">
+        <v>157</v>
+      </c>
+      <c r="S50" s="4">
+        <v>5.5469999999999997</v>
+      </c>
+      <c r="T50" s="4">
+        <v>332.04300000000001</v>
+      </c>
+    </row>
+    <row r="51" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N51" t="s">
+        <v>154</v>
+      </c>
+      <c r="O51" s="2">
+        <v>42557</v>
+      </c>
+      <c r="P51" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q51">
+        <v>2</v>
+      </c>
+      <c r="R51" t="s">
+        <v>157</v>
+      </c>
+      <c r="S51" s="4">
+        <v>5.7629999999999999</v>
+      </c>
+      <c r="T51" s="4">
+        <v>325.755</v>
+      </c>
+    </row>
+    <row r="52" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N52" t="s">
+        <v>154</v>
+      </c>
+      <c r="O52" s="2">
+        <v>42557</v>
+      </c>
+      <c r="P52" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q52">
+        <v>1</v>
+      </c>
+      <c r="R52" t="s">
+        <v>166</v>
+      </c>
+      <c r="S52" s="4">
+        <v>6.8280000000000003</v>
+      </c>
+      <c r="T52" s="4">
+        <v>339.75099999999998</v>
+      </c>
+    </row>
+    <row r="53" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N53" t="s">
+        <v>154</v>
+      </c>
+      <c r="O53" s="2">
+        <v>42557</v>
+      </c>
+      <c r="P53" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q53">
+        <v>2</v>
+      </c>
+      <c r="R53" t="s">
+        <v>166</v>
+      </c>
+      <c r="S53" s="4">
+        <v>7.5380000000000003</v>
+      </c>
+      <c r="T53" s="4">
+        <v>360.15199999999999</v>
+      </c>
+    </row>
+    <row r="54" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N54" t="s">
+        <v>154</v>
+      </c>
+      <c r="O54" s="2">
+        <v>42557</v>
+      </c>
+      <c r="P54" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q54">
+        <v>1</v>
+      </c>
+      <c r="R54" t="s">
+        <v>157</v>
+      </c>
+      <c r="S54" s="4">
+        <v>4.1760000000000002</v>
+      </c>
+      <c r="T54" s="4">
+        <v>368.88200000000001</v>
+      </c>
+    </row>
+    <row r="55" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N55" t="s">
+        <v>154</v>
+      </c>
+      <c r="O55" s="2">
+        <v>42557</v>
+      </c>
+      <c r="P55" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q55">
+        <v>2</v>
+      </c>
+      <c r="R55" t="s">
+        <v>157</v>
+      </c>
+      <c r="S55" s="4">
+        <v>4.7190000000000003</v>
+      </c>
+      <c r="T55" s="4">
+        <v>352.87799999999999</v>
+      </c>
+    </row>
+    <row r="56" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N56" t="s">
+        <v>154</v>
+      </c>
+      <c r="O56" s="2">
+        <v>42557</v>
+      </c>
+      <c r="P56" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q56">
+        <v>1</v>
+      </c>
+      <c r="R56" t="s">
+        <v>166</v>
+      </c>
+      <c r="S56" s="4">
+        <v>5.1509999999999998</v>
+      </c>
+      <c r="T56" s="4">
+        <v>388.601</v>
+      </c>
+    </row>
+    <row r="57" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N57" t="s">
+        <v>154</v>
+      </c>
+      <c r="O57" s="2">
+        <v>42557</v>
+      </c>
+      <c r="P57" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q57">
+        <v>2</v>
+      </c>
+      <c r="R57" t="s">
+        <v>166</v>
+      </c>
+      <c r="S57" s="4">
+        <v>9.4600000000000009</v>
+      </c>
+      <c r="T57" s="4">
+        <v>425.73599999999999</v>
+      </c>
+    </row>
+    <row r="58" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N58" t="s">
+        <v>154</v>
+      </c>
+      <c r="O58" s="2">
+        <v>42557</v>
+      </c>
+      <c r="P58" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q58">
+        <v>1</v>
+      </c>
+      <c r="R58" t="s">
+        <v>157</v>
+      </c>
+      <c r="S58" s="4">
+        <v>4.8780000000000001</v>
+      </c>
+      <c r="T58" s="4">
+        <v>337.63900000000001</v>
+      </c>
+    </row>
+    <row r="59" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N59" t="s">
+        <v>154</v>
+      </c>
+      <c r="O59" s="2">
+        <v>42557</v>
+      </c>
+      <c r="P59" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q59">
+        <v>2</v>
+      </c>
+      <c r="R59" t="s">
+        <v>157</v>
+      </c>
+      <c r="S59" s="4">
+        <v>5.3170000000000002</v>
+      </c>
+      <c r="T59" s="4">
+        <v>339.92899999999997</v>
+      </c>
+    </row>
+    <row r="60" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N60" t="s">
+        <v>154</v>
+      </c>
+      <c r="O60" s="2">
+        <v>42557</v>
+      </c>
+      <c r="P60" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q60">
+        <v>1</v>
+      </c>
+      <c r="R60" t="s">
+        <v>166</v>
+      </c>
+      <c r="S60" s="4">
+        <v>4.33</v>
+      </c>
+      <c r="T60" s="4">
+        <v>334.93299999999999</v>
+      </c>
+    </row>
+    <row r="61" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N61" t="s">
+        <v>154</v>
+      </c>
+      <c r="O61" s="2">
+        <v>42557</v>
+      </c>
+      <c r="P61" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q61">
+        <v>2</v>
+      </c>
+      <c r="R61" t="s">
+        <v>166</v>
+      </c>
+      <c r="S61" s="4">
+        <v>8.0350000000000001</v>
+      </c>
+      <c r="T61" s="4">
+        <v>482.505</v>
+      </c>
+    </row>
+    <row r="62" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N62" t="s">
+        <v>154</v>
+      </c>
+      <c r="O62" s="2">
+        <v>42557</v>
+      </c>
+      <c r="P62" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q62">
+        <v>1</v>
+      </c>
+      <c r="R62" t="s">
+        <v>157</v>
+      </c>
+      <c r="S62" s="4">
+        <v>6.569</v>
+      </c>
+      <c r="T62" s="4">
+        <v>278.12400000000002</v>
+      </c>
+    </row>
+    <row r="63" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N63" t="s">
+        <v>154</v>
+      </c>
+      <c r="O63" s="2">
+        <v>42557</v>
+      </c>
+      <c r="P63" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q63">
+        <v>2</v>
+      </c>
+      <c r="R63" t="s">
+        <v>157</v>
+      </c>
+      <c r="S63" s="4">
+        <v>6.1580000000000004</v>
+      </c>
+      <c r="T63" s="4">
+        <v>265.10700000000003</v>
+      </c>
+    </row>
+    <row r="64" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N64" t="s">
+        <v>154</v>
+      </c>
+      <c r="O64" s="2">
+        <v>42557</v>
+      </c>
+      <c r="P64" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q64">
+        <v>1</v>
+      </c>
+      <c r="R64" t="s">
+        <v>166</v>
+      </c>
+      <c r="S64" s="4">
+        <v>5.532</v>
+      </c>
+      <c r="T64" s="4">
+        <v>253.726</v>
+      </c>
+    </row>
+    <row r="65" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N65" t="s">
+        <v>154</v>
+      </c>
+      <c r="O65" s="2">
+        <v>42557</v>
+      </c>
+      <c r="P65" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q65">
+        <v>2</v>
+      </c>
+      <c r="R65" t="s">
+        <v>166</v>
+      </c>
+      <c r="S65" s="4">
+        <v>3.9940000000000002</v>
+      </c>
+      <c r="T65" s="4">
+        <v>240.26300000000001</v>
+      </c>
+    </row>
+    <row r="66" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N66" t="s">
+        <v>154</v>
+      </c>
+      <c r="O66" s="2">
+        <v>42557</v>
+      </c>
+      <c r="P66" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q66">
+        <v>1</v>
+      </c>
+      <c r="R66" t="s">
+        <v>157</v>
+      </c>
+      <c r="S66" s="4">
+        <v>5.3659999999999997</v>
+      </c>
+      <c r="T66" s="4">
+        <v>285.358</v>
+      </c>
+    </row>
+    <row r="67" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N67" t="s">
+        <v>154</v>
+      </c>
+      <c r="O67" s="2">
+        <v>42557</v>
+      </c>
+      <c r="P67" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q67">
+        <v>2</v>
+      </c>
+      <c r="R67" t="s">
+        <v>157</v>
+      </c>
+      <c r="S67" s="4">
+        <v>4.165</v>
+      </c>
+      <c r="T67" s="4">
+        <v>284.79700000000003</v>
+      </c>
+    </row>
+    <row r="68" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N68" t="s">
+        <v>154</v>
+      </c>
+      <c r="O68" s="2">
+        <v>42557</v>
+      </c>
+      <c r="P68" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q68">
+        <v>1</v>
+      </c>
+      <c r="R68" t="s">
+        <v>166</v>
+      </c>
+      <c r="S68" s="4">
+        <v>7.1989999999999998</v>
+      </c>
+      <c r="T68" s="4">
+        <v>451.375</v>
+      </c>
+    </row>
+    <row r="69" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N69" t="s">
+        <v>154</v>
+      </c>
+      <c r="O69" s="2">
+        <v>42557</v>
+      </c>
+      <c r="P69" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q69">
+        <v>2</v>
+      </c>
+      <c r="R69" t="s">
+        <v>166</v>
+      </c>
+      <c r="S69" s="4">
+        <v>9.0419999999999998</v>
+      </c>
+      <c r="T69" s="4">
+        <v>556.39099999999996</v>
+      </c>
+    </row>
+    <row r="70" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N70" t="s">
+        <v>154</v>
+      </c>
+      <c r="O70" s="2">
+        <v>42558</v>
+      </c>
+      <c r="P70" t="s">
+        <v>164</v>
+      </c>
+      <c r="Q70">
+        <v>1</v>
+      </c>
+      <c r="R70" t="s">
+        <v>157</v>
+      </c>
+      <c r="S70" s="4">
+        <v>7.8339999999999996</v>
+      </c>
+      <c r="T70" s="4">
+        <v>386.85899999999998</v>
+      </c>
+    </row>
+    <row r="71" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N71" t="s">
+        <v>154</v>
+      </c>
+      <c r="O71" s="2">
+        <v>42558</v>
+      </c>
+      <c r="P71" t="s">
+        <v>164</v>
+      </c>
+      <c r="Q71">
+        <v>2</v>
+      </c>
+      <c r="R71" t="s">
+        <v>157</v>
+      </c>
+      <c r="S71" s="4">
+        <v>5.6539999999999999</v>
+      </c>
+      <c r="T71" s="4">
+        <v>356.94</v>
+      </c>
+    </row>
+    <row r="72" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N72" t="s">
+        <v>154</v>
+      </c>
+      <c r="O72" s="2">
+        <v>42558</v>
+      </c>
+      <c r="P72" t="s">
+        <v>164</v>
+      </c>
+      <c r="Q72">
+        <v>1</v>
+      </c>
+      <c r="R72" t="s">
+        <v>166</v>
+      </c>
+      <c r="S72" s="4">
+        <v>6.7869999999999999</v>
+      </c>
+      <c r="T72" s="4">
+        <v>373.64100000000002</v>
+      </c>
+    </row>
+    <row r="73" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N73" t="s">
+        <v>154</v>
+      </c>
+      <c r="O73" s="2">
+        <v>42558</v>
+      </c>
+      <c r="P73" t="s">
+        <v>164</v>
+      </c>
+      <c r="Q73">
+        <v>2</v>
+      </c>
+      <c r="R73" t="s">
+        <v>166</v>
+      </c>
+      <c r="S73" s="4">
+        <v>6.4450000000000003</v>
+      </c>
+      <c r="T73" s="4">
+        <v>377.32400000000001</v>
+      </c>
+    </row>
+    <row r="74" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N74" t="s">
+        <v>154</v>
+      </c>
+      <c r="O74" s="2">
+        <v>42558</v>
+      </c>
+      <c r="P74" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q74">
+        <v>1</v>
+      </c>
+      <c r="R74" t="s">
+        <v>157</v>
+      </c>
+      <c r="S74" s="4">
+        <v>6.3559999999999999</v>
+      </c>
+      <c r="T74" s="4">
+        <v>324.38900000000001</v>
+      </c>
+    </row>
+    <row r="75" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N75" t="s">
+        <v>154</v>
+      </c>
+      <c r="O75" s="2">
+        <v>42558</v>
+      </c>
+      <c r="P75" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q75">
+        <v>2</v>
+      </c>
+      <c r="R75" t="s">
+        <v>157</v>
+      </c>
+      <c r="S75" s="4">
+        <v>7.3369999999999997</v>
+      </c>
+      <c r="T75" s="4">
+        <v>339.07900000000001</v>
+      </c>
+    </row>
+    <row r="76" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N76" t="s">
+        <v>154</v>
+      </c>
+      <c r="O76" s="2">
+        <v>42558</v>
+      </c>
+      <c r="P76" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q76">
+        <v>1</v>
+      </c>
+      <c r="R76" t="s">
+        <v>166</v>
+      </c>
+      <c r="S76" s="4">
+        <v>7.1769999999999996</v>
+      </c>
+      <c r="T76" s="4">
+        <v>307.14299999999997</v>
+      </c>
+    </row>
+    <row r="77" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N77" t="s">
+        <v>154</v>
+      </c>
+      <c r="O77" s="2">
+        <v>42558</v>
+      </c>
+      <c r="P77" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q77">
+        <v>2</v>
+      </c>
+      <c r="R77" t="s">
+        <v>166</v>
+      </c>
+      <c r="S77" s="4">
+        <v>6.8490000000000002</v>
+      </c>
+      <c r="T77" s="4">
+        <v>302.55700000000002</v>
+      </c>
+    </row>
+    <row r="78" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N78" t="s">
+        <v>154</v>
+      </c>
+      <c r="O78" s="2">
+        <v>42558</v>
+      </c>
+      <c r="P78" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q78">
+        <v>1</v>
+      </c>
+      <c r="R78" t="s">
+        <v>157</v>
+      </c>
+      <c r="S78" s="4">
+        <v>5.6970000000000001</v>
+      </c>
+      <c r="T78" s="4">
+        <v>287.06700000000001</v>
+      </c>
+    </row>
+    <row r="79" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N79" t="s">
+        <v>154</v>
+      </c>
+      <c r="O79" s="2">
+        <v>42558</v>
+      </c>
+      <c r="P79" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q79">
+        <v>2</v>
+      </c>
+      <c r="R79" t="s">
+        <v>157</v>
+      </c>
+      <c r="S79" s="4">
+        <v>4.5780000000000003</v>
+      </c>
+      <c r="T79" s="4">
+        <v>273.666</v>
+      </c>
+    </row>
+    <row r="80" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N80" t="s">
+        <v>154</v>
+      </c>
+      <c r="O80" s="2">
+        <v>42558</v>
+      </c>
+      <c r="P80" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q80">
+        <v>1</v>
+      </c>
+      <c r="R80" t="s">
+        <v>166</v>
+      </c>
+      <c r="S80" s="4">
+        <v>5.1459999999999999</v>
+      </c>
+      <c r="T80" s="4">
+        <v>293.57600000000002</v>
+      </c>
+    </row>
+    <row r="81" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N81" t="s">
+        <v>154</v>
+      </c>
+      <c r="O81" s="2">
+        <v>42558</v>
+      </c>
+      <c r="P81" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q81">
+        <v>2</v>
+      </c>
+      <c r="R81" t="s">
+        <v>166</v>
+      </c>
+      <c r="S81" s="4">
+        <v>9.766</v>
+      </c>
+      <c r="T81" s="4">
+        <v>372.66500000000002</v>
+      </c>
+    </row>
+    <row r="82" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N82" t="s">
+        <v>154</v>
+      </c>
+      <c r="O82" s="2">
+        <v>42558</v>
+      </c>
+      <c r="P82" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q82">
+        <v>1</v>
+      </c>
+      <c r="R82" t="s">
+        <v>157</v>
+      </c>
+      <c r="S82" s="4">
+        <v>6.1669999999999998</v>
+      </c>
+      <c r="T82" s="4">
+        <v>248.82</v>
+      </c>
+    </row>
+    <row r="83" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N83" t="s">
+        <v>154</v>
+      </c>
+      <c r="O83" s="2">
+        <v>42558</v>
+      </c>
+      <c r="P83" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q83">
+        <v>2</v>
+      </c>
+      <c r="R83" t="s">
+        <v>157</v>
+      </c>
+      <c r="S83" s="4">
+        <v>5.048</v>
+      </c>
+      <c r="T83" s="4">
+        <v>251.92</v>
+      </c>
+    </row>
+    <row r="84" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N84" t="s">
+        <v>154</v>
+      </c>
+      <c r="O84" s="2">
+        <v>42558</v>
+      </c>
+      <c r="P84" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q84">
+        <v>1</v>
+      </c>
+      <c r="R84" t="s">
+        <v>166</v>
+      </c>
+      <c r="S84" s="4">
+        <v>6.0670000000000002</v>
+      </c>
+      <c r="T84" s="4">
+        <v>285.42200000000003</v>
+      </c>
+    </row>
+    <row r="85" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N85" t="s">
+        <v>154</v>
+      </c>
+      <c r="O85" s="2">
+        <v>42558</v>
+      </c>
+      <c r="P85" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q85">
+        <v>2</v>
+      </c>
+      <c r="R85" t="s">
+        <v>166</v>
+      </c>
+      <c r="S85" s="4">
+        <v>4.6420000000000003</v>
+      </c>
+      <c r="T85" s="4">
+        <v>265.42</v>
+      </c>
+    </row>
+    <row r="86" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N86" t="s">
+        <v>154</v>
+      </c>
+      <c r="O86" s="2">
+        <v>42558</v>
+      </c>
+      <c r="P86" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q86">
+        <v>1</v>
+      </c>
+      <c r="R86" t="s">
+        <v>157</v>
+      </c>
+      <c r="S86" s="4">
+        <v>2.0379999999999998</v>
+      </c>
+      <c r="T86" s="4">
+        <v>237.55699999999999</v>
+      </c>
+    </row>
+    <row r="87" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N87" t="s">
+        <v>154</v>
+      </c>
+      <c r="O87" s="2">
+        <v>42558</v>
+      </c>
+      <c r="P87" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q87">
+        <v>2</v>
+      </c>
+      <c r="R87" t="s">
+        <v>157</v>
+      </c>
+      <c r="S87" s="4">
+        <v>1.9350000000000001</v>
+      </c>
+      <c r="T87" s="4">
+        <v>220.55199999999999</v>
+      </c>
+    </row>
+    <row r="88" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N88" t="s">
+        <v>154</v>
+      </c>
+      <c r="O88" s="2">
+        <v>42558</v>
+      </c>
+      <c r="P88" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q88">
+        <v>1</v>
+      </c>
+      <c r="R88" t="s">
+        <v>166</v>
+      </c>
+      <c r="S88" s="4">
+        <v>5.3890000000000002</v>
+      </c>
+      <c r="T88" s="4">
+        <v>253.61600000000001</v>
+      </c>
+    </row>
+    <row r="89" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N89" t="s">
+        <v>154</v>
+      </c>
+      <c r="O89" s="2">
+        <v>42558</v>
+      </c>
+      <c r="P89" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q89">
+        <v>2</v>
+      </c>
+      <c r="R89" t="s">
+        <v>166</v>
+      </c>
+      <c r="S89" s="4">
+        <v>4.3</v>
+      </c>
+      <c r="T89" s="4">
+        <v>243.88</v>
+      </c>
+    </row>
+    <row r="90" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N90" t="s">
+        <v>154</v>
+      </c>
+      <c r="O90" s="2">
+        <v>42558</v>
+      </c>
+      <c r="P90" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q90">
+        <v>1</v>
+      </c>
+      <c r="R90" t="s">
+        <v>157</v>
+      </c>
+      <c r="S90" s="4">
+        <v>7.02</v>
+      </c>
+      <c r="T90" s="4">
+        <v>316.70800000000003</v>
+      </c>
+    </row>
+    <row r="91" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N91" t="s">
+        <v>154</v>
+      </c>
+      <c r="O91" s="2">
+        <v>42558</v>
+      </c>
+      <c r="P91" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q91">
+        <v>2</v>
+      </c>
+      <c r="R91" t="s">
+        <v>157</v>
+      </c>
+      <c r="S91" s="4">
+        <v>6.8929999999999998</v>
+      </c>
+      <c r="T91" s="4">
+        <v>321.50099999999998</v>
+      </c>
+    </row>
+    <row r="92" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N92" t="s">
+        <v>154</v>
+      </c>
+      <c r="O92" s="2">
+        <v>42558</v>
+      </c>
+      <c r="P92" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q92">
+        <v>1</v>
+      </c>
+      <c r="R92" t="s">
+        <v>166</v>
+      </c>
+      <c r="S92" s="4">
+        <v>5.8040000000000003</v>
+      </c>
+      <c r="T92" s="4">
+        <v>390.89600000000002</v>
+      </c>
+    </row>
+    <row r="93" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N93" t="s">
+        <v>154</v>
+      </c>
+      <c r="O93" s="2">
+        <v>42558</v>
+      </c>
+      <c r="P93" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q93">
+        <v>2</v>
+      </c>
+      <c r="R93" t="s">
+        <v>166</v>
+      </c>
+      <c r="S93" s="4">
+        <v>6.2949999999999999</v>
+      </c>
+      <c r="T93" s="4">
+        <v>322.49200000000002</v>
+      </c>
+    </row>
+    <row r="94" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N94" t="s">
+        <v>154</v>
+      </c>
+      <c r="O94" s="2">
+        <v>42560</v>
+      </c>
+      <c r="P94" t="s">
+        <v>164</v>
+      </c>
+      <c r="Q94">
+        <v>1</v>
+      </c>
+      <c r="R94" t="s">
+        <v>157</v>
+      </c>
+      <c r="S94" s="4">
+        <v>5.3319999999999999</v>
+      </c>
+      <c r="T94" s="4">
+        <v>319.45</v>
+      </c>
+    </row>
+    <row r="95" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N95" t="s">
+        <v>154</v>
+      </c>
+      <c r="O95" s="2">
+        <v>42560</v>
+      </c>
+      <c r="P95" t="s">
+        <v>164</v>
+      </c>
+      <c r="Q95">
+        <v>2</v>
+      </c>
+      <c r="R95" t="s">
+        <v>157</v>
+      </c>
+      <c r="S95" s="4">
+        <v>4.3730000000000002</v>
+      </c>
+      <c r="T95" s="4">
+        <v>316.45299999999997</v>
+      </c>
+    </row>
+    <row r="96" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N96" t="s">
+        <v>154</v>
+      </c>
+      <c r="O96" s="2">
+        <v>42560</v>
+      </c>
+      <c r="P96" t="s">
+        <v>164</v>
+      </c>
+      <c r="Q96">
+        <v>1</v>
+      </c>
+      <c r="R96" t="s">
+        <v>166</v>
+      </c>
+      <c r="S96" s="4">
+        <v>6.4710000000000001</v>
+      </c>
+      <c r="T96" s="4">
+        <v>343.43700000000001</v>
+      </c>
+    </row>
+    <row r="97" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N97" t="s">
+        <v>154</v>
+      </c>
+      <c r="O97" s="2">
+        <v>42560</v>
+      </c>
+      <c r="P97" t="s">
+        <v>164</v>
+      </c>
+      <c r="Q97">
+        <v>2</v>
+      </c>
+      <c r="R97" t="s">
+        <v>166</v>
+      </c>
+      <c r="S97" s="4">
+        <v>7.407</v>
+      </c>
+      <c r="T97" s="4">
+        <v>340.17099999999999</v>
+      </c>
+    </row>
+    <row r="98" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N98" t="s">
+        <v>155</v>
+      </c>
+      <c r="O98" s="2">
+        <v>42559</v>
+      </c>
+      <c r="P98" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q98">
+        <v>1</v>
+      </c>
+      <c r="R98" t="s">
+        <v>157</v>
+      </c>
+      <c r="S98" s="4">
+        <v>15.08</v>
+      </c>
+      <c r="T98" s="4">
+        <v>536.00199999999995</v>
+      </c>
+    </row>
+    <row r="99" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N99" t="s">
+        <v>155</v>
+      </c>
+      <c r="O99" s="2">
+        <v>42559</v>
+      </c>
+      <c r="P99" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q99">
+        <v>2</v>
+      </c>
+      <c r="R99" t="s">
+        <v>157</v>
+      </c>
+      <c r="S99" s="4">
+        <v>13.87</v>
+      </c>
+      <c r="T99" s="4">
+        <v>567.15800000000002</v>
+      </c>
+    </row>
+    <row r="100" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N100" t="s">
+        <v>155</v>
+      </c>
+      <c r="O100" s="2">
+        <v>42559</v>
+      </c>
+      <c r="P100" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q100">
+        <v>1</v>
+      </c>
+      <c r="R100" t="s">
+        <v>166</v>
+      </c>
+      <c r="S100" s="4">
+        <v>20.257999999999999</v>
+      </c>
+      <c r="T100" s="4">
+        <v>604.91899999999998</v>
+      </c>
+    </row>
+    <row r="101" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N101" t="s">
+        <v>155</v>
+      </c>
+      <c r="O101" s="2">
+        <v>42559</v>
+      </c>
+      <c r="P101" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q101">
+        <v>2</v>
+      </c>
+      <c r="R101" t="s">
+        <v>166</v>
+      </c>
+      <c r="S101" s="4">
+        <v>18.018999999999998</v>
+      </c>
+      <c r="T101" s="4">
+        <v>598.053</v>
+      </c>
+    </row>
+    <row r="102" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N102" t="s">
+        <v>155</v>
+      </c>
+      <c r="O102" s="2">
+        <v>42559</v>
+      </c>
+      <c r="P102" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q102">
+        <v>1</v>
+      </c>
+      <c r="R102" t="s">
+        <v>157</v>
+      </c>
+      <c r="S102" s="4">
+        <v>14.637</v>
+      </c>
+      <c r="T102" s="4">
+        <v>537.81899999999996</v>
+      </c>
+    </row>
+    <row r="103" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N103" t="s">
+        <v>155</v>
+      </c>
+      <c r="O103" s="2">
+        <v>42559</v>
+      </c>
+      <c r="P103" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q103">
+        <v>2</v>
+      </c>
+      <c r="R103" t="s">
+        <v>157</v>
+      </c>
+      <c r="S103" s="4">
+        <v>11.571</v>
+      </c>
+      <c r="T103" s="4">
+        <v>565.33500000000004</v>
+      </c>
+    </row>
+    <row r="104" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N104" t="s">
+        <v>155</v>
+      </c>
+      <c r="O104" s="2">
+        <v>42559</v>
+      </c>
+      <c r="P104" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q104">
+        <v>1</v>
+      </c>
+      <c r="R104" t="s">
+        <v>166</v>
+      </c>
+      <c r="S104" s="4">
+        <v>26.324999999999999</v>
+      </c>
+      <c r="T104" s="4">
+        <v>700.13800000000003</v>
+      </c>
+    </row>
+    <row r="105" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N105" t="s">
+        <v>155</v>
+      </c>
+      <c r="O105" s="2">
+        <v>42559</v>
+      </c>
+      <c r="P105" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q105">
+        <v>2</v>
+      </c>
+      <c r="R105" t="s">
+        <v>166</v>
+      </c>
+      <c r="S105" s="4">
+        <v>27.606000000000002</v>
+      </c>
+      <c r="T105" s="4">
+        <v>713.92899999999997</v>
+      </c>
+    </row>
+    <row r="106" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N106" t="s">
+        <v>155</v>
+      </c>
+      <c r="O106" s="2">
+        <v>42559</v>
+      </c>
+      <c r="P106" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q106">
+        <v>1</v>
+      </c>
+      <c r="R106" t="s">
+        <v>157</v>
+      </c>
+      <c r="S106" s="4">
+        <v>14.045999999999999</v>
+      </c>
+      <c r="T106" s="4">
+        <v>620.41800000000001</v>
+      </c>
+    </row>
+    <row r="107" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N107" t="s">
+        <v>155</v>
+      </c>
+      <c r="O107" s="2">
+        <v>42559</v>
+      </c>
+      <c r="P107" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q107">
+        <v>2</v>
+      </c>
+      <c r="R107" t="s">
+        <v>157</v>
+      </c>
+      <c r="S107" s="4">
+        <v>14.625</v>
+      </c>
+      <c r="T107" s="4">
+        <v>565.42100000000005</v>
+      </c>
+    </row>
+    <row r="108" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N108" t="s">
+        <v>155</v>
+      </c>
+      <c r="O108" s="2">
+        <v>42559</v>
+      </c>
+      <c r="P108" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q108">
+        <v>1</v>
+      </c>
+      <c r="R108" t="s">
+        <v>166</v>
+      </c>
+      <c r="S108" s="4">
+        <v>29.247</v>
+      </c>
+      <c r="T108" s="4">
+        <v>720.71799999999996</v>
+      </c>
+    </row>
+    <row r="109" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N109" t="s">
+        <v>155</v>
+      </c>
+      <c r="O109" s="2">
+        <v>42559</v>
+      </c>
+      <c r="P109" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q109">
+        <v>2</v>
+      </c>
+      <c r="R109" t="s">
+        <v>166</v>
+      </c>
+      <c r="S109" s="4">
+        <v>31.957999999999998</v>
+      </c>
+      <c r="T109" s="4">
+        <v>736.13400000000001</v>
+      </c>
+    </row>
+    <row r="110" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N110" t="s">
+        <v>155</v>
+      </c>
+      <c r="O110" s="2">
+        <v>42559</v>
+      </c>
+      <c r="P110" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q110">
+        <v>1</v>
+      </c>
+      <c r="R110" t="s">
+        <v>157</v>
+      </c>
+      <c r="S110" s="4">
+        <v>14.614000000000001</v>
+      </c>
+      <c r="T110" s="4">
+        <v>614.13499999999999</v>
+      </c>
+    </row>
+    <row r="111" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N111" t="s">
+        <v>155</v>
+      </c>
+      <c r="O111" s="2">
+        <v>42559</v>
+      </c>
+      <c r="P111" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q111">
+        <v>2</v>
+      </c>
+      <c r="R111" t="s">
+        <v>157</v>
+      </c>
+      <c r="S111" s="4">
+        <v>16.498000000000001</v>
+      </c>
+      <c r="T111" s="4">
+        <v>598.73599999999999</v>
+      </c>
+    </row>
+    <row r="112" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N112" t="s">
+        <v>155</v>
+      </c>
+      <c r="O112" s="2">
+        <v>42559</v>
+      </c>
+      <c r="P112" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q112">
+        <v>1</v>
+      </c>
+      <c r="R112" t="s">
+        <v>166</v>
+      </c>
+      <c r="S112" s="4">
+        <v>28.058</v>
+      </c>
+      <c r="T112" s="4">
+        <v>671.10199999999998</v>
+      </c>
+    </row>
+    <row r="113" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N113" t="s">
+        <v>155</v>
+      </c>
+      <c r="O113" s="2">
+        <v>42559</v>
+      </c>
+      <c r="P113" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q113">
+        <v>2</v>
+      </c>
+      <c r="R113" t="s">
+        <v>166</v>
+      </c>
+      <c r="S113" s="4">
+        <v>18.004000000000001</v>
+      </c>
+      <c r="T113" s="4">
+        <v>612.46100000000001</v>
+      </c>
+    </row>
+    <row r="114" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N114" t="s">
+        <v>155</v>
+      </c>
+      <c r="O114" s="2">
+        <v>42559</v>
+      </c>
+      <c r="P114" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q114">
+        <v>1</v>
+      </c>
+      <c r="R114" t="s">
+        <v>157</v>
+      </c>
+      <c r="S114" s="4">
+        <v>15.177</v>
+      </c>
+      <c r="T114" s="4">
+        <v>553.31399999999996</v>
+      </c>
+    </row>
+    <row r="115" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N115" t="s">
+        <v>155</v>
+      </c>
+      <c r="O115" s="2">
+        <v>42559</v>
+      </c>
+      <c r="P115" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q115">
+        <v>2</v>
+      </c>
+      <c r="R115" t="s">
+        <v>157</v>
+      </c>
+      <c r="S115" s="4">
+        <v>15.803000000000001</v>
+      </c>
+      <c r="T115" s="4">
+        <v>554.88</v>
+      </c>
+    </row>
+    <row r="116" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N116" t="s">
+        <v>155</v>
+      </c>
+      <c r="O116" s="2">
+        <v>42559</v>
+      </c>
+      <c r="P116" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q116">
+        <v>1</v>
+      </c>
+      <c r="R116" t="s">
+        <v>166</v>
+      </c>
+      <c r="S116" s="4">
+        <v>20.317</v>
+      </c>
+      <c r="T116" s="4">
+        <v>649.93200000000002</v>
+      </c>
+    </row>
+    <row r="117" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N117" t="s">
+        <v>155</v>
+      </c>
+      <c r="O117" s="2">
+        <v>42559</v>
+      </c>
+      <c r="P117" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q117">
+        <v>2</v>
+      </c>
+      <c r="R117" t="s">
+        <v>166</v>
+      </c>
+      <c r="S117" s="4">
+        <v>16.384</v>
+      </c>
+      <c r="T117" s="4">
+        <v>591.26599999999996</v>
+      </c>
+    </row>
+    <row r="118" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N118" t="s">
+        <v>155</v>
+      </c>
+      <c r="O118" s="2">
+        <v>42560</v>
+      </c>
+      <c r="P118" t="s">
+        <v>164</v>
+      </c>
+      <c r="Q118">
+        <v>1</v>
+      </c>
+      <c r="R118" t="s">
+        <v>157</v>
+      </c>
+      <c r="S118" s="4">
+        <v>16.695</v>
+      </c>
+      <c r="T118" s="4">
+        <v>580.23800000000006</v>
+      </c>
+    </row>
+    <row r="119" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N119" t="s">
+        <v>155</v>
+      </c>
+      <c r="O119" s="2">
+        <v>42560</v>
+      </c>
+      <c r="P119" t="s">
+        <v>164</v>
+      </c>
+      <c r="Q119">
+        <v>2</v>
+      </c>
+      <c r="R119" t="s">
+        <v>157</v>
+      </c>
+      <c r="S119" s="4">
+        <v>13.911</v>
+      </c>
+      <c r="T119" s="4">
+        <v>600.97900000000004</v>
+      </c>
+    </row>
+    <row r="120" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N120" t="s">
+        <v>155</v>
+      </c>
+      <c r="O120" s="2">
+        <v>42560</v>
+      </c>
+      <c r="P120" t="s">
+        <v>164</v>
+      </c>
+      <c r="Q120">
+        <v>1</v>
+      </c>
+      <c r="R120" t="s">
+        <v>166</v>
+      </c>
+      <c r="S120" s="4">
+        <v>15.099</v>
+      </c>
+      <c r="T120" s="4">
+        <v>623.61900000000003</v>
+      </c>
+    </row>
+    <row r="121" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N121" t="s">
+        <v>155</v>
+      </c>
+      <c r="O121" s="2">
+        <v>42560</v>
+      </c>
+      <c r="P121" t="s">
+        <v>164</v>
+      </c>
+      <c r="Q121">
+        <v>2</v>
+      </c>
+      <c r="R121" t="s">
+        <v>166</v>
+      </c>
+      <c r="S121" s="4">
+        <v>23.844000000000001</v>
+      </c>
+      <c r="T121" s="4">
+        <v>702.11300000000006</v>
+      </c>
+    </row>
+    <row r="122" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N122" t="s">
+        <v>155</v>
+      </c>
+      <c r="O122" s="2">
+        <v>42560</v>
+      </c>
+      <c r="P122" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q122">
+        <v>1</v>
+      </c>
+      <c r="R122" t="s">
+        <v>157</v>
+      </c>
+      <c r="S122" s="4">
+        <v>17.125</v>
+      </c>
+      <c r="T122" s="4">
+        <v>599.726</v>
+      </c>
+    </row>
+    <row r="123" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N123" t="s">
+        <v>155</v>
+      </c>
+      <c r="O123" s="2">
+        <v>42560</v>
+      </c>
+      <c r="P123" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q123">
+        <v>2</v>
+      </c>
+      <c r="R123" t="s">
+        <v>157</v>
+      </c>
+      <c r="S123" s="4">
+        <v>15.25</v>
+      </c>
+      <c r="T123" s="4">
+        <v>552.74599999999998</v>
+      </c>
+    </row>
+    <row r="124" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N124" t="s">
+        <v>155</v>
+      </c>
+      <c r="O124" s="2">
+        <v>42560</v>
+      </c>
+      <c r="P124" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q124">
+        <v>1</v>
+      </c>
+      <c r="R124" t="s">
+        <v>166</v>
+      </c>
+      <c r="S124" s="4">
+        <v>16.585999999999999</v>
+      </c>
+      <c r="T124" s="4">
+        <v>603.85</v>
+      </c>
+    </row>
+    <row r="125" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N125" t="s">
+        <v>155</v>
+      </c>
+      <c r="O125" s="2">
+        <v>42560</v>
+      </c>
+      <c r="P125" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q125">
+        <v>2</v>
+      </c>
+      <c r="R125" t="s">
+        <v>166</v>
+      </c>
+      <c r="S125" s="4">
+        <v>18.437999999999999</v>
+      </c>
+      <c r="T125" s="4">
+        <v>607.41200000000003</v>
+      </c>
+    </row>
+    <row r="126" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N126" t="s">
+        <v>155</v>
+      </c>
+      <c r="O126" s="2">
+        <v>42560</v>
+      </c>
+      <c r="P126" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q126">
+        <v>1</v>
+      </c>
+      <c r="R126" t="s">
+        <v>157</v>
+      </c>
+      <c r="S126" s="4">
+        <v>21.896999999999998</v>
+      </c>
+      <c r="T126" s="4">
+        <v>557.78399999999999</v>
+      </c>
+    </row>
+    <row r="127" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N127" t="s">
+        <v>155</v>
+      </c>
+      <c r="O127" s="2">
+        <v>42560</v>
+      </c>
+      <c r="P127" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q127">
+        <v>2</v>
+      </c>
+      <c r="R127" t="s">
+        <v>157</v>
+      </c>
+      <c r="S127" s="4">
+        <v>20.867000000000001</v>
+      </c>
+      <c r="T127" s="4">
+        <v>601.40700000000004</v>
+      </c>
+    </row>
+    <row r="128" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N128" t="s">
+        <v>155</v>
+      </c>
+      <c r="O128" s="2">
+        <v>42560</v>
+      </c>
+      <c r="P128" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q128">
+        <v>1</v>
+      </c>
+      <c r="R128" t="s">
+        <v>166</v>
+      </c>
+      <c r="S128" s="4">
+        <v>23.751000000000001</v>
+      </c>
+      <c r="T128" s="4">
+        <v>658.15599999999995</v>
+      </c>
+    </row>
+    <row r="129" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N129" t="s">
+        <v>155</v>
+      </c>
+      <c r="O129" s="2">
+        <v>42560</v>
+      </c>
+      <c r="P129" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q129">
+        <v>2</v>
+      </c>
+      <c r="R129" t="s">
+        <v>166</v>
+      </c>
+      <c r="S129" s="4">
+        <v>26.366</v>
+      </c>
+      <c r="T129" s="4">
+        <v>698.62300000000005</v>
+      </c>
+    </row>
+    <row r="130" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N130" t="s">
+        <v>155</v>
+      </c>
+      <c r="O130" s="2">
+        <v>42560</v>
+      </c>
+      <c r="P130" t="s">
+        <v>164</v>
+      </c>
+      <c r="Q130">
+        <v>1</v>
+      </c>
+      <c r="R130" t="s">
+        <v>157</v>
+      </c>
+      <c r="S130" s="4">
+        <v>14.429</v>
+      </c>
+      <c r="T130" s="4">
+        <v>684.39800000000002</v>
+      </c>
+    </row>
+    <row r="131" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N131" t="s">
+        <v>155</v>
+      </c>
+      <c r="O131" s="2">
+        <v>42560</v>
+      </c>
+      <c r="P131" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q131">
+        <v>2</v>
+      </c>
+      <c r="R131" t="s">
+        <v>157</v>
+      </c>
+      <c r="S131" s="4">
+        <v>13.281000000000001</v>
+      </c>
+      <c r="T131" s="4">
+        <v>656.971</v>
+      </c>
+    </row>
+    <row r="132" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N132" t="s">
+        <v>155</v>
+      </c>
+      <c r="O132" s="2">
+        <v>42560</v>
+      </c>
+      <c r="P132" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q132">
+        <v>1</v>
+      </c>
+      <c r="R132" t="s">
+        <v>166</v>
+      </c>
+      <c r="S132" s="4">
+        <v>33.229999999999997</v>
+      </c>
+      <c r="T132" s="4">
+        <v>812.01400000000001</v>
+      </c>
+    </row>
+    <row r="133" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N133" t="s">
+        <v>155</v>
+      </c>
+      <c r="O133" s="2">
+        <v>42560</v>
+      </c>
+      <c r="P133" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q133">
+        <v>2</v>
+      </c>
+      <c r="R133" t="s">
+        <v>166</v>
+      </c>
+      <c r="S133" s="4">
+        <v>27.706</v>
+      </c>
+      <c r="T133" s="4">
+        <v>733.98599999999999</v>
+      </c>
+    </row>
+    <row r="134" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N134" t="s">
+        <v>155</v>
+      </c>
+      <c r="O134" s="2">
+        <v>42560</v>
+      </c>
+      <c r="P134" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q134">
+        <v>1</v>
+      </c>
+      <c r="R134" t="s">
+        <v>157</v>
+      </c>
+      <c r="S134" s="4">
+        <v>12.446999999999999</v>
+      </c>
+      <c r="T134" s="4">
+        <v>616.60900000000004</v>
+      </c>
+    </row>
+    <row r="135" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N135" t="s">
+        <v>155</v>
+      </c>
+      <c r="O135" s="2">
+        <v>42560</v>
+      </c>
+      <c r="P135" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q135">
+        <v>2</v>
+      </c>
+      <c r="R135" t="s">
+        <v>157</v>
+      </c>
+      <c r="S135" s="4">
+        <v>12.634</v>
+      </c>
+      <c r="T135" s="4">
+        <v>647.70399999999995</v>
+      </c>
+    </row>
+    <row r="136" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N136" t="s">
+        <v>155</v>
+      </c>
+      <c r="O136" s="2">
+        <v>42560</v>
+      </c>
+      <c r="P136" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q136">
+        <v>1</v>
+      </c>
+      <c r="R136" t="s">
+        <v>166</v>
+      </c>
+      <c r="S136" s="4">
+        <v>23.128</v>
+      </c>
+      <c r="T136" s="4">
+        <v>699.20899999999995</v>
+      </c>
+    </row>
+    <row r="137" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N137" t="s">
+        <v>155</v>
+      </c>
+      <c r="O137" s="2">
+        <v>42560</v>
+      </c>
+      <c r="P137" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q137">
+        <v>2</v>
+      </c>
+      <c r="R137" t="s">
+        <v>166</v>
+      </c>
+      <c r="S137" s="4">
+        <v>25.699000000000002</v>
+      </c>
+      <c r="T137" s="4">
+        <v>685.72400000000005</v>
+      </c>
+    </row>
+    <row r="138" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N138" t="s">
+        <v>155</v>
+      </c>
+      <c r="O138" s="2">
+        <v>42560</v>
+      </c>
+      <c r="P138" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q138">
+        <v>1</v>
+      </c>
+      <c r="R138" t="s">
+        <v>157</v>
+      </c>
+      <c r="S138" s="4">
+        <v>16.486000000000001</v>
+      </c>
+      <c r="T138" s="4">
+        <v>564.49400000000003</v>
+      </c>
+    </row>
+    <row r="139" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N139" t="s">
+        <v>155</v>
+      </c>
+      <c r="O139" s="2">
+        <v>42560</v>
+      </c>
+      <c r="P139" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q139">
+        <v>2</v>
+      </c>
+      <c r="R139" t="s">
+        <v>157</v>
+      </c>
+      <c r="S139" s="4">
+        <v>15.699</v>
+      </c>
+      <c r="T139" s="4">
+        <v>570.13099999999997</v>
+      </c>
+    </row>
+    <row r="140" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N140" t="s">
+        <v>155</v>
+      </c>
+      <c r="O140" s="2">
+        <v>42560</v>
+      </c>
+      <c r="P140" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q140">
+        <v>1</v>
+      </c>
+      <c r="R140" t="s">
+        <v>166</v>
+      </c>
+      <c r="S140" s="4">
+        <v>20.771000000000001</v>
+      </c>
+      <c r="T140" s="4">
+        <v>630.41999999999996</v>
+      </c>
+    </row>
+    <row r="141" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N141" t="s">
+        <v>155</v>
+      </c>
+      <c r="O141" s="2">
+        <v>42560</v>
+      </c>
+      <c r="P141" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q141">
+        <v>2</v>
+      </c>
+      <c r="R141" t="s">
+        <v>166</v>
+      </c>
+      <c r="S141" s="4">
+        <v>21.384</v>
+      </c>
+      <c r="T141" s="4">
+        <v>717.84699999999998</v>
+      </c>
+    </row>
+    <row r="142" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N142" t="s">
+        <v>155</v>
+      </c>
+      <c r="O142" s="2">
+        <v>42561</v>
+      </c>
+      <c r="P142" t="s">
+        <v>164</v>
+      </c>
+      <c r="Q142">
+        <v>1</v>
+      </c>
+      <c r="R142" t="s">
+        <v>157</v>
+      </c>
+      <c r="S142" s="4">
+        <v>13.061999999999999</v>
+      </c>
+      <c r="T142" s="4">
+        <v>588.44500000000005</v>
+      </c>
+    </row>
+    <row r="143" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N143" t="s">
+        <v>155</v>
+      </c>
+      <c r="O143" s="2">
+        <v>42561</v>
+      </c>
+      <c r="P143" t="s">
+        <v>164</v>
+      </c>
+      <c r="Q143">
+        <v>2</v>
+      </c>
+      <c r="R143" t="s">
+        <v>157</v>
+      </c>
+      <c r="S143" s="4">
+        <v>13.428000000000001</v>
+      </c>
+      <c r="T143" s="4">
+        <v>571.63900000000001</v>
+      </c>
+    </row>
+    <row r="144" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N144" t="s">
+        <v>155</v>
+      </c>
+      <c r="O144" s="2">
+        <v>42561</v>
+      </c>
+      <c r="P144" t="s">
+        <v>164</v>
+      </c>
+      <c r="Q144">
+        <v>1</v>
+      </c>
+      <c r="R144" t="s">
+        <v>166</v>
+      </c>
+      <c r="S144" s="4">
+        <v>18.321000000000002</v>
+      </c>
+      <c r="T144" s="4">
+        <v>613.00699999999995</v>
+      </c>
+    </row>
+    <row r="145" spans="14:20" x14ac:dyDescent="0.25">
+      <c r="N145" t="s">
+        <v>155</v>
+      </c>
+      <c r="O145" s="2">
+        <v>42561</v>
+      </c>
+      <c r="P145" t="s">
+        <v>164</v>
+      </c>
+      <c r="Q145">
+        <v>2</v>
+      </c>
+      <c r="R145" t="s">
+        <v>166</v>
+      </c>
+      <c r="S145" s="4">
+        <v>18.163</v>
+      </c>
+      <c r="T145" s="4">
+        <v>636.55999999999995</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Finished uploading nitrogen and phosphorus measurements to LIMs. Finished extracting CDS regions from Sparkling MGs and reran that, started the clustering to run overnight.
</commit_message>
<xml_diff>
--- a/environmental_data/for_humans/Copy of GEODES_TNTP.xlsx
+++ b/environmental_data/for_humans/Copy of GEODES_TNTP.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1070" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="202">
   <si>
     <t>F/SP_7-6_5AM1</t>
   </si>
@@ -627,12 +627,6 @@
   </si>
   <si>
     <t>GEODES_TB_44hr</t>
-  </si>
-  <si>
-    <t>TN/TDN and TP/TDP are the averages of 2 replicates each.</t>
-  </si>
-  <si>
-    <t>Cyanotoxins measured by Todd Miller's lab.</t>
   </si>
 </sst>
 </file>
@@ -5998,18 +5992,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:U145"/>
+  <dimension ref="A1:T33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U2" sqref="U2:U3"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.7109375" customWidth="1"/>
     <col min="6" max="6" width="4.28515625" customWidth="1"/>
-    <col min="7" max="10" width="9.140625" style="4"/>
-    <col min="11" max="13" width="2.7109375" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="4" customWidth="1"/>
+    <col min="8" max="10" width="9.140625" style="4"/>
+    <col min="11" max="11" width="7" customWidth="1"/>
+    <col min="12" max="12" width="12.7109375" customWidth="1"/>
+    <col min="13" max="13" width="11.85546875" customWidth="1"/>
     <col min="14" max="14" width="5" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="9.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="6.7109375" bestFit="1" customWidth="1"/>
@@ -6019,7 +6016,7 @@
     <col min="20" max="20" width="7.7109375" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>167</v>
       </c>
@@ -6035,3580 +6032,550 @@
       <c r="E1" t="s">
         <v>169</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="N1" t="s">
-        <v>149</v>
-      </c>
-      <c r="O1" t="s">
-        <v>153</v>
-      </c>
-      <c r="P1" t="s">
-        <v>150</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>165</v>
-      </c>
-      <c r="R1" t="s">
-        <v>158</v>
-      </c>
-      <c r="S1" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="T1" s="4" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="O1"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>170</v>
       </c>
-      <c r="G2" s="4">
-        <f>AVERAGE(T4:T5)</f>
+      <c r="B2">
         <v>616.59699999999998</v>
       </c>
-      <c r="H2" s="4">
-        <f>AVERAGE(S4:S5)</f>
+      <c r="C2">
         <v>18.738999999999997</v>
       </c>
-      <c r="I2" s="4">
-        <f>AVERAGE(T2:T3)</f>
+      <c r="D2">
         <v>500.24849999999998</v>
       </c>
-      <c r="J2" s="4">
-        <f>AVERAGE(S2:S3)</f>
+      <c r="E2">
         <v>7.8554999999999993</v>
       </c>
-      <c r="N2" t="s">
-        <v>156</v>
-      </c>
-      <c r="O2" s="2">
-        <v>42565</v>
-      </c>
-      <c r="P2" t="s">
-        <v>159</v>
-      </c>
-      <c r="Q2">
-        <v>1</v>
-      </c>
-      <c r="R2" t="s">
-        <v>157</v>
-      </c>
-      <c r="S2" s="4">
-        <v>8.0139999999999993</v>
-      </c>
-      <c r="T2" s="4">
-        <v>518.15499999999997</v>
-      </c>
-      <c r="U2" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>171</v>
       </c>
-      <c r="G3" s="4">
-        <f>AVERAGE(T16:T17)</f>
+      <c r="B3">
         <v>713.89850000000001</v>
       </c>
-      <c r="H3" s="4">
-        <f>AVERAGE(S16:S17)</f>
+      <c r="C3">
         <v>19.43</v>
       </c>
-      <c r="I3" s="4">
-        <f>AVERAGE(T14:T15)</f>
+      <c r="D3">
         <v>509.00850000000003</v>
       </c>
-      <c r="J3" s="4">
-        <f>AVERAGE(S14:S15)</f>
+      <c r="E3">
         <v>9.2100000000000009</v>
       </c>
-      <c r="N3" t="s">
-        <v>156</v>
-      </c>
-      <c r="O3" s="2">
-        <v>42565</v>
-      </c>
-      <c r="P3" t="s">
-        <v>159</v>
-      </c>
-      <c r="Q3">
-        <v>2</v>
-      </c>
-      <c r="R3" t="s">
-        <v>157</v>
-      </c>
-      <c r="S3" s="4">
-        <v>7.6970000000000001</v>
-      </c>
-      <c r="T3" s="4">
-        <v>482.34199999999998</v>
-      </c>
-      <c r="U3" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>172</v>
       </c>
-      <c r="G4" s="4">
-        <f>AVERAGE(T20:T21)</f>
+      <c r="B4">
         <v>618.98299999999995</v>
       </c>
-      <c r="H4" s="4">
-        <f>AVERAGE(S20:S21)</f>
+      <c r="C4">
         <v>18.357500000000002</v>
       </c>
-      <c r="I4" s="4">
-        <f>AVERAGE(T18:T19)</f>
+      <c r="D4">
         <v>507.726</v>
       </c>
-      <c r="J4" s="4">
-        <f>AVERAGE(S18:S19)</f>
+      <c r="E4">
         <v>9.7949999999999999</v>
       </c>
-      <c r="N4" t="s">
-        <v>156</v>
-      </c>
-      <c r="O4" s="2">
-        <v>42565</v>
-      </c>
-      <c r="P4" t="s">
-        <v>159</v>
-      </c>
-      <c r="Q4">
-        <v>1</v>
-      </c>
-      <c r="R4" t="s">
-        <v>166</v>
-      </c>
-      <c r="S4" s="4">
-        <v>18.835999999999999</v>
-      </c>
-      <c r="T4" s="4">
-        <v>591.36699999999996</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>173</v>
       </c>
-      <c r="G5" s="4">
-        <f>AVERAGE(T24:T25)</f>
+      <c r="B5">
         <v>662.30449999999996</v>
       </c>
-      <c r="H5" s="4">
-        <f>AVERAGE(S24:S25)</f>
+      <c r="C5">
         <v>22.120999999999999</v>
       </c>
-      <c r="I5" s="4">
-        <f>AVERAGE(T22:T23)</f>
+      <c r="D5">
         <v>508.37599999999998</v>
       </c>
-      <c r="J5" s="4">
-        <f>AVERAGE(S22:S23)</f>
+      <c r="E5">
         <v>8.7585000000000015</v>
       </c>
-      <c r="N5" t="s">
-        <v>156</v>
-      </c>
-      <c r="O5" s="2">
-        <v>42565</v>
-      </c>
-      <c r="P5" t="s">
-        <v>159</v>
-      </c>
-      <c r="Q5">
-        <v>2</v>
-      </c>
-      <c r="R5" t="s">
-        <v>166</v>
-      </c>
-      <c r="S5" s="4">
-        <v>18.641999999999999</v>
-      </c>
-      <c r="T5" s="4">
-        <v>641.827</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>174</v>
       </c>
-      <c r="G6" s="4">
-        <f>AVERAGE(T28:T29)</f>
+      <c r="B6">
         <v>592.33749999999998</v>
       </c>
-      <c r="H6" s="4">
-        <f>AVERAGE(S28:S29)</f>
+      <c r="C6">
         <v>18.023499999999999</v>
       </c>
-      <c r="I6" s="4">
-        <f>AVERAGE(T26:T27)</f>
+      <c r="D6">
         <v>470.13</v>
       </c>
-      <c r="J6" s="4">
-        <f>AVERAGE(S26:S27)</f>
+      <c r="E6">
         <v>7.0404999999999998</v>
       </c>
-      <c r="N6" t="s">
-        <v>156</v>
-      </c>
-      <c r="O6" s="2">
-        <v>42565</v>
-      </c>
-      <c r="P6" t="s">
-        <v>160</v>
-      </c>
-      <c r="Q6">
-        <v>1</v>
-      </c>
-      <c r="R6" t="s">
-        <v>157</v>
-      </c>
-      <c r="S6" s="4">
-        <v>10.257999999999999</v>
-      </c>
-      <c r="T6" s="4">
-        <v>566.66300000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>175</v>
       </c>
-      <c r="G7" s="4">
-        <f>AVERAGE(T32:T33)</f>
+      <c r="B7">
         <v>623.79349999999999</v>
       </c>
-      <c r="H7" s="4">
-        <f>AVERAGE(S32:S33)</f>
+      <c r="C7">
         <v>19.7105</v>
       </c>
-      <c r="I7" s="4">
-        <f>AVERAGE(T30:T31)</f>
+      <c r="D7">
         <v>507.19499999999999</v>
       </c>
-      <c r="J7" s="4">
-        <f>AVERAGE(S30:S31)</f>
+      <c r="E7">
         <v>9.4700000000000006</v>
       </c>
-      <c r="N7" t="s">
-        <v>156</v>
-      </c>
-      <c r="O7" s="2">
-        <v>42565</v>
-      </c>
-      <c r="P7" t="s">
-        <v>160</v>
-      </c>
-      <c r="Q7">
-        <v>2</v>
-      </c>
-      <c r="R7" t="s">
-        <v>157</v>
-      </c>
-      <c r="S7" s="4">
-        <v>10.488</v>
-      </c>
-      <c r="T7" s="4">
-        <v>531.00900000000001</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>176</v>
       </c>
-      <c r="G8" s="4">
-        <f>AVERAGE(T36:T37)</f>
+      <c r="B8">
         <v>580.84799999999996</v>
       </c>
-      <c r="H8" s="4">
-        <f>AVERAGE(S36:S37)</f>
+      <c r="C8">
         <v>15.785500000000001</v>
       </c>
-      <c r="I8" s="4">
-        <f>AVERAGE(T34:T35)</f>
+      <c r="D8">
         <v>517.39499999999998</v>
       </c>
-      <c r="J8" s="4">
-        <f>AVERAGE(S34:S35)</f>
+      <c r="E8">
         <v>8.1509999999999998</v>
       </c>
-      <c r="N8" t="s">
-        <v>156</v>
-      </c>
-      <c r="O8" s="2">
-        <v>42565</v>
-      </c>
-      <c r="P8" t="s">
-        <v>160</v>
-      </c>
-      <c r="Q8">
-        <v>1</v>
-      </c>
-      <c r="R8" t="s">
-        <v>166</v>
-      </c>
-      <c r="S8" s="4">
-        <v>18.885999999999999</v>
-      </c>
-      <c r="T8" s="4">
-        <v>671.48</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>177</v>
       </c>
-      <c r="G9" s="4">
-        <f>AVERAGE(T40:T41)</f>
+      <c r="B9">
         <v>586.37950000000001</v>
       </c>
-      <c r="H9" s="4">
-        <f>AVERAGE(S40:S41)</f>
+      <c r="C9">
         <v>17.075500000000002</v>
       </c>
-      <c r="I9" s="4">
-        <f>AVERAGE(T38:T39)</f>
+      <c r="D9">
         <v>500.005</v>
       </c>
-      <c r="J9" s="4">
-        <f>AVERAGE(S38:S39)</f>
+      <c r="E9">
         <v>8.7684999999999995</v>
       </c>
-      <c r="N9" t="s">
-        <v>156</v>
-      </c>
-      <c r="O9" s="2">
-        <v>42565</v>
-      </c>
-      <c r="P9" t="s">
-        <v>160</v>
-      </c>
-      <c r="Q9">
-        <v>2</v>
-      </c>
-      <c r="R9" t="s">
-        <v>166</v>
-      </c>
-      <c r="S9" s="4">
-        <v>20.881</v>
-      </c>
-      <c r="T9" s="4">
-        <v>658.71600000000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>178</v>
       </c>
-      <c r="N10" t="s">
-        <v>156</v>
-      </c>
-      <c r="O10" s="2">
-        <v>42565</v>
-      </c>
-      <c r="P10" t="s">
-        <v>161</v>
-      </c>
-      <c r="Q10">
-        <v>1</v>
-      </c>
-      <c r="R10" t="s">
-        <v>157</v>
-      </c>
-      <c r="S10" s="4">
-        <v>8.4969999999999999</v>
-      </c>
-      <c r="T10" s="4">
-        <v>513.42399999999998</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>665.09799999999996</v>
+      </c>
+      <c r="C10">
+        <v>19.883499999999998</v>
+      </c>
+      <c r="D10">
+        <v>548.83600000000001</v>
+      </c>
+      <c r="E10">
+        <v>10.372999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>179</v>
       </c>
-      <c r="N11" t="s">
-        <v>156</v>
-      </c>
-      <c r="O11" s="2">
-        <v>42565</v>
-      </c>
-      <c r="P11" t="s">
-        <v>161</v>
-      </c>
-      <c r="Q11">
-        <v>2</v>
-      </c>
-      <c r="R11" t="s">
-        <v>157</v>
-      </c>
-      <c r="S11" s="4">
-        <v>9.2780000000000005</v>
-      </c>
-      <c r="T11" s="4">
-        <v>482.673</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>598.09500000000003</v>
+      </c>
+      <c r="C11">
+        <v>19.009999999999998</v>
+      </c>
+      <c r="D11">
+        <v>498.04849999999999</v>
+      </c>
+      <c r="E11">
+        <v>8.8874999999999993</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>180</v>
       </c>
-      <c r="N12" t="s">
-        <v>156</v>
-      </c>
-      <c r="O12" s="2">
-        <v>42565</v>
-      </c>
-      <c r="P12" t="s">
-        <v>161</v>
-      </c>
-      <c r="Q12">
-        <v>1</v>
-      </c>
-      <c r="R12" t="s">
-        <v>166</v>
-      </c>
-      <c r="S12" s="4">
-        <v>17.805</v>
-      </c>
-      <c r="T12" s="4">
-        <v>578.44200000000001</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>349.95150000000001</v>
+      </c>
+      <c r="C12">
+        <v>7.1829999999999998</v>
+      </c>
+      <c r="D12">
+        <v>328.899</v>
+      </c>
+      <c r="E12">
+        <v>5.6549999999999994</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>181</v>
       </c>
-      <c r="N13" t="s">
-        <v>156</v>
-      </c>
-      <c r="O13" s="2">
-        <v>42565</v>
-      </c>
-      <c r="P13" t="s">
-        <v>161</v>
-      </c>
-      <c r="Q13">
-        <v>2</v>
-      </c>
-      <c r="R13" t="s">
-        <v>166</v>
-      </c>
-      <c r="S13" s="4">
-        <v>20.215</v>
-      </c>
-      <c r="T13" s="4">
-        <v>617.74800000000005</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>246.99450000000002</v>
+      </c>
+      <c r="C13">
+        <v>4.7629999999999999</v>
+      </c>
+      <c r="D13">
+        <v>271.6155</v>
+      </c>
+      <c r="E13">
+        <v>6.3635000000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>182</v>
       </c>
-      <c r="N14" t="s">
-        <v>156</v>
-      </c>
-      <c r="O14" s="2">
-        <v>42565</v>
-      </c>
-      <c r="P14" t="s">
-        <v>162</v>
-      </c>
-      <c r="Q14">
-        <v>1</v>
-      </c>
-      <c r="R14" t="s">
-        <v>157</v>
-      </c>
-      <c r="S14" s="4">
-        <v>9.7309999999999999</v>
-      </c>
-      <c r="T14" s="4">
-        <v>512.10400000000004</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>503.88299999999998</v>
+      </c>
+      <c r="C14">
+        <v>8.1204999999999998</v>
+      </c>
+      <c r="D14">
+        <v>285.07749999999999</v>
+      </c>
+      <c r="E14">
+        <v>4.7654999999999994</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>183</v>
       </c>
-      <c r="N15" t="s">
-        <v>156</v>
-      </c>
-      <c r="O15" s="2">
-        <v>42565</v>
-      </c>
-      <c r="P15" t="s">
-        <v>162</v>
-      </c>
-      <c r="Q15">
-        <v>2</v>
-      </c>
-      <c r="R15" t="s">
-        <v>157</v>
-      </c>
-      <c r="S15" s="4">
-        <v>8.6890000000000001</v>
-      </c>
-      <c r="T15" s="4">
-        <v>505.91300000000001</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>375.48250000000002</v>
+      </c>
+      <c r="C15">
+        <v>6.6159999999999997</v>
+      </c>
+      <c r="D15">
+        <v>371.89949999999999</v>
+      </c>
+      <c r="E15">
+        <v>6.7439999999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>184</v>
       </c>
-      <c r="N16" t="s">
-        <v>156</v>
-      </c>
-      <c r="O16" s="2">
-        <v>42565</v>
-      </c>
-      <c r="P16" t="s">
-        <v>162</v>
-      </c>
-      <c r="Q16">
-        <v>1</v>
-      </c>
-      <c r="R16" t="s">
-        <v>166</v>
-      </c>
-      <c r="S16" s="4">
-        <v>18.341000000000001</v>
-      </c>
-      <c r="T16" s="4">
-        <v>665.55799999999999</v>
-      </c>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>304.85000000000002</v>
+      </c>
+      <c r="C16">
+        <v>7.0129999999999999</v>
+      </c>
+      <c r="D16">
+        <v>331.73400000000004</v>
+      </c>
+      <c r="E16">
+        <v>6.8464999999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>185</v>
       </c>
-      <c r="N17" t="s">
-        <v>156</v>
-      </c>
-      <c r="O17" s="2">
-        <v>42565</v>
-      </c>
-      <c r="P17" t="s">
-        <v>162</v>
-      </c>
-      <c r="Q17">
-        <v>2</v>
-      </c>
-      <c r="R17" t="s">
-        <v>166</v>
-      </c>
-      <c r="S17" s="4">
-        <v>20.518999999999998</v>
-      </c>
-      <c r="T17" s="4">
-        <v>762.23900000000003</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>333.12049999999999</v>
+      </c>
+      <c r="C17">
+        <v>7.4559999999999995</v>
+      </c>
+      <c r="D17">
+        <v>280.36649999999997</v>
+      </c>
+      <c r="E17">
+        <v>5.1375000000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>186</v>
       </c>
-      <c r="N18" t="s">
-        <v>156</v>
-      </c>
-      <c r="O18" s="2">
-        <v>42565</v>
-      </c>
-      <c r="P18" t="s">
-        <v>163</v>
-      </c>
-      <c r="Q18">
-        <v>1</v>
-      </c>
-      <c r="R18" t="s">
-        <v>157</v>
-      </c>
-      <c r="S18" s="4">
-        <v>9.9559999999999995</v>
-      </c>
-      <c r="T18" s="4">
-        <v>520.96299999999997</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>275.42100000000005</v>
+      </c>
+      <c r="C18">
+        <v>5.3544999999999998</v>
+      </c>
+      <c r="D18">
+        <v>250.37</v>
+      </c>
+      <c r="E18">
+        <v>5.6074999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>187</v>
       </c>
-      <c r="N19" t="s">
-        <v>156</v>
-      </c>
-      <c r="O19" s="2">
-        <v>42565</v>
-      </c>
-      <c r="P19" t="s">
-        <v>163</v>
-      </c>
-      <c r="Q19">
-        <v>2</v>
-      </c>
-      <c r="R19" t="s">
-        <v>157</v>
-      </c>
-      <c r="S19" s="4">
-        <v>9.6340000000000003</v>
-      </c>
-      <c r="T19" s="4">
-        <v>494.48899999999998</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>248.74799999999999</v>
+      </c>
+      <c r="C19">
+        <v>4.8445</v>
+      </c>
+      <c r="D19">
+        <v>229.05449999999999</v>
+      </c>
+      <c r="E19">
+        <v>1.9864999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>190</v>
       </c>
-      <c r="N20" t="s">
-        <v>156</v>
-      </c>
-      <c r="O20" s="2">
-        <v>42565</v>
-      </c>
-      <c r="P20" t="s">
-        <v>163</v>
-      </c>
-      <c r="Q20">
-        <v>1</v>
-      </c>
-      <c r="R20" t="s">
-        <v>166</v>
-      </c>
-      <c r="S20" s="4">
-        <v>17.975999999999999</v>
-      </c>
-      <c r="T20" s="4">
-        <v>617.21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>356.69400000000002</v>
+      </c>
+      <c r="C20">
+        <v>6.0495000000000001</v>
+      </c>
+      <c r="D20">
+        <v>319.10450000000003</v>
+      </c>
+      <c r="E20">
+        <v>6.9565000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>188</v>
       </c>
-      <c r="N21" t="s">
-        <v>156</v>
-      </c>
-      <c r="O21" s="2">
-        <v>42565</v>
-      </c>
-      <c r="P21" t="s">
-        <v>163</v>
-      </c>
-      <c r="Q21">
-        <v>2</v>
-      </c>
-      <c r="R21" t="s">
-        <v>166</v>
-      </c>
-      <c r="S21" s="4">
-        <v>18.739000000000001</v>
-      </c>
-      <c r="T21" s="4">
-        <v>620.75599999999997</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>407.16849999999999</v>
+      </c>
+      <c r="C21">
+        <v>7.3055000000000003</v>
+      </c>
+      <c r="D21">
+        <v>349.95150000000001</v>
+      </c>
+      <c r="E21">
+        <v>4.4474999999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>189</v>
       </c>
-      <c r="N22" t="s">
-        <v>156</v>
-      </c>
-      <c r="O22" s="2">
-        <v>42566</v>
-      </c>
-      <c r="P22" t="s">
-        <v>164</v>
-      </c>
-      <c r="Q22">
-        <v>1</v>
-      </c>
-      <c r="R22" t="s">
-        <v>157</v>
-      </c>
-      <c r="S22" s="4">
-        <v>8.6240000000000006</v>
-      </c>
-      <c r="T22" s="4">
-        <v>506.33800000000002</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>408.71899999999999</v>
+      </c>
+      <c r="C22">
+        <v>6.1825000000000001</v>
+      </c>
+      <c r="D22">
+        <v>338.78399999999999</v>
+      </c>
+      <c r="E22">
+        <v>5.0975000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>191</v>
       </c>
-      <c r="N23" t="s">
-        <v>156</v>
-      </c>
-      <c r="O23" s="2">
-        <v>42566</v>
-      </c>
-      <c r="P23" t="s">
-        <v>164</v>
-      </c>
-      <c r="Q23">
-        <v>2</v>
-      </c>
-      <c r="R23" t="s">
-        <v>157</v>
-      </c>
-      <c r="S23" s="4">
-        <v>8.8930000000000007</v>
-      </c>
-      <c r="T23" s="4">
-        <v>510.41399999999999</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>601.48599999999999</v>
+      </c>
+      <c r="C23">
+        <v>19.138500000000001</v>
+      </c>
+      <c r="D23">
+        <v>551.57999999999993</v>
+      </c>
+      <c r="E23">
+        <v>14.475</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>192</v>
       </c>
-      <c r="N24" t="s">
-        <v>156</v>
-      </c>
-      <c r="O24" s="2">
-        <v>42566</v>
-      </c>
-      <c r="P24" t="s">
-        <v>164</v>
-      </c>
-      <c r="Q24">
-        <v>1</v>
-      </c>
-      <c r="R24" t="s">
-        <v>166</v>
-      </c>
-      <c r="S24" s="4">
-        <v>21.254999999999999</v>
-      </c>
-      <c r="T24" s="4">
-        <v>672.173</v>
-      </c>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>641.78150000000005</v>
+      </c>
+      <c r="C24">
+        <v>23.030999999999999</v>
+      </c>
+      <c r="D24">
+        <v>606.43550000000005</v>
+      </c>
+      <c r="E24">
+        <v>15.556000000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>193</v>
       </c>
-      <c r="N25" t="s">
-        <v>156</v>
-      </c>
-      <c r="O25" s="2">
-        <v>42566</v>
-      </c>
-      <c r="P25" t="s">
-        <v>164</v>
-      </c>
-      <c r="Q25">
-        <v>2</v>
-      </c>
-      <c r="R25" t="s">
-        <v>166</v>
-      </c>
-      <c r="S25" s="4">
-        <v>22.986999999999998</v>
-      </c>
-      <c r="T25" s="4">
-        <v>652.43600000000004</v>
-      </c>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>620.59899999999993</v>
+      </c>
+      <c r="C25">
+        <v>18.3505</v>
+      </c>
+      <c r="D25">
+        <v>554.09699999999998</v>
+      </c>
+      <c r="E25">
+        <v>15.49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>194</v>
       </c>
-      <c r="N26" t="s">
-        <v>156</v>
-      </c>
-      <c r="O26" s="2">
-        <v>42566</v>
-      </c>
-      <c r="P26" t="s">
-        <v>159</v>
-      </c>
-      <c r="Q26">
-        <v>1</v>
-      </c>
-      <c r="R26" t="s">
-        <v>157</v>
-      </c>
-      <c r="S26" s="4">
-        <v>6.24</v>
-      </c>
-      <c r="T26" s="4">
-        <v>470.41399999999999</v>
-      </c>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>605.63100000000009</v>
+      </c>
+      <c r="C26">
+        <v>17.512</v>
+      </c>
+      <c r="D26">
+        <v>576.23599999999999</v>
+      </c>
+      <c r="E26">
+        <v>19.471499999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>195</v>
       </c>
-      <c r="N27" t="s">
-        <v>156</v>
-      </c>
-      <c r="O27" s="2">
-        <v>42566</v>
-      </c>
-      <c r="P27" t="s">
-        <v>159</v>
-      </c>
-      <c r="Q27">
-        <v>2</v>
-      </c>
-      <c r="R27" t="s">
-        <v>157</v>
-      </c>
-      <c r="S27" s="4">
-        <v>7.8410000000000002</v>
-      </c>
-      <c r="T27" s="4">
-        <v>469.846</v>
-      </c>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>678.3895</v>
+      </c>
+      <c r="C27">
+        <v>25.058500000000002</v>
+      </c>
+      <c r="D27">
+        <v>579.59550000000002</v>
+      </c>
+      <c r="E27">
+        <v>21.381999999999998</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>196</v>
       </c>
-      <c r="N28" t="s">
-        <v>156</v>
-      </c>
-      <c r="O28" s="2">
-        <v>42566</v>
-      </c>
-      <c r="P28" t="s">
-        <v>159</v>
-      </c>
-      <c r="Q28">
-        <v>1</v>
-      </c>
-      <c r="R28" t="s">
-        <v>166</v>
-      </c>
-      <c r="S28" s="4">
-        <v>14.407</v>
-      </c>
-      <c r="T28" s="4">
-        <v>572.92999999999995</v>
-      </c>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <v>773</v>
+      </c>
+      <c r="C28">
+        <v>30.467999999999996</v>
+      </c>
+      <c r="D28">
+        <v>670.68450000000007</v>
+      </c>
+      <c r="E28">
+        <v>13.855</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>197</v>
       </c>
-      <c r="N29" t="s">
-        <v>156</v>
-      </c>
-      <c r="O29" s="2">
-        <v>42566</v>
-      </c>
-      <c r="P29" t="s">
-        <v>159</v>
-      </c>
-      <c r="Q29">
-        <v>2</v>
-      </c>
-      <c r="R29" t="s">
-        <v>166</v>
-      </c>
-      <c r="S29" s="4">
-        <v>21.64</v>
-      </c>
-      <c r="T29" s="4">
-        <v>611.745</v>
-      </c>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <v>692.4665</v>
+      </c>
+      <c r="C29">
+        <v>24.413499999999999</v>
+      </c>
+      <c r="D29">
+        <v>632.15650000000005</v>
+      </c>
+      <c r="E29">
+        <v>12.5405</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>198</v>
       </c>
-      <c r="N30" t="s">
-        <v>156</v>
-      </c>
-      <c r="O30" s="2">
-        <v>42566</v>
-      </c>
-      <c r="P30" t="s">
-        <v>160</v>
-      </c>
-      <c r="Q30">
-        <v>1</v>
-      </c>
-      <c r="R30" t="s">
-        <v>157</v>
-      </c>
-      <c r="S30" s="4">
-        <v>9.1620000000000008</v>
-      </c>
-      <c r="T30" s="4">
-        <v>502.839</v>
-      </c>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>674.13349999999991</v>
+      </c>
+      <c r="C30">
+        <v>21.077500000000001</v>
+      </c>
+      <c r="D30">
+        <v>567.3125</v>
+      </c>
+      <c r="E30">
+        <v>16.092500000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>201</v>
       </c>
-      <c r="N31" t="s">
-        <v>156</v>
-      </c>
-      <c r="O31" s="2">
-        <v>42566</v>
-      </c>
-      <c r="P31" t="s">
-        <v>160</v>
-      </c>
-      <c r="Q31">
-        <v>2</v>
-      </c>
-      <c r="R31" t="s">
-        <v>157</v>
-      </c>
-      <c r="S31" s="4">
-        <v>9.7780000000000005</v>
-      </c>
-      <c r="T31" s="4">
-        <v>511.55099999999999</v>
-      </c>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <v>624.7835</v>
+      </c>
+      <c r="C31">
+        <v>18.242000000000001</v>
+      </c>
+      <c r="D31">
+        <v>580.04200000000003</v>
+      </c>
+      <c r="E31">
+        <v>13.245000000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>199</v>
       </c>
-      <c r="N32" t="s">
-        <v>156</v>
-      </c>
-      <c r="O32" s="2">
-        <v>42566</v>
-      </c>
-      <c r="P32" t="s">
-        <v>160</v>
-      </c>
-      <c r="Q32">
-        <v>1</v>
-      </c>
-      <c r="R32" t="s">
-        <v>166</v>
-      </c>
-      <c r="S32" s="4">
-        <v>22.827999999999999</v>
-      </c>
-      <c r="T32" s="4">
-        <v>644.05399999999997</v>
-      </c>
-    </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <v>707.0335</v>
+      </c>
+      <c r="C32">
+        <v>26.965499999999999</v>
+      </c>
+      <c r="D32">
+        <v>551.577</v>
+      </c>
+      <c r="E32">
+        <v>13.103999999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>200</v>
       </c>
-      <c r="N33" t="s">
-        <v>156</v>
-      </c>
-      <c r="O33" s="2">
-        <v>42566</v>
-      </c>
-      <c r="P33" t="s">
-        <v>160</v>
-      </c>
-      <c r="Q33">
-        <v>2</v>
-      </c>
-      <c r="R33" t="s">
-        <v>166</v>
-      </c>
-      <c r="S33" s="4">
-        <v>16.593</v>
-      </c>
-      <c r="T33" s="4">
-        <v>603.53300000000002</v>
-      </c>
-    </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="N34" t="s">
-        <v>156</v>
-      </c>
-      <c r="O34" s="2">
-        <v>42566</v>
-      </c>
-      <c r="P34" t="s">
-        <v>161</v>
-      </c>
-      <c r="Q34">
-        <v>1</v>
-      </c>
-      <c r="R34" t="s">
-        <v>157</v>
-      </c>
-      <c r="S34" s="4">
-        <v>8.3140000000000001</v>
-      </c>
-      <c r="T34" s="4">
-        <v>504.55900000000003</v>
-      </c>
-    </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="N35" t="s">
-        <v>156</v>
-      </c>
-      <c r="O35" s="2">
-        <v>42566</v>
-      </c>
-      <c r="P35" t="s">
-        <v>161</v>
-      </c>
-      <c r="Q35">
-        <v>2</v>
-      </c>
-      <c r="R35" t="s">
-        <v>157</v>
-      </c>
-      <c r="S35" s="4">
-        <v>7.9880000000000004</v>
-      </c>
-      <c r="T35" s="4">
-        <v>530.23099999999999</v>
-      </c>
-    </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="N36" t="s">
-        <v>156</v>
-      </c>
-      <c r="O36" s="2">
-        <v>42566</v>
-      </c>
-      <c r="P36" t="s">
-        <v>161</v>
-      </c>
-      <c r="Q36">
-        <v>1</v>
-      </c>
-      <c r="R36" t="s">
-        <v>166</v>
-      </c>
-      <c r="S36" s="4">
-        <v>16.315000000000001</v>
-      </c>
-      <c r="T36" s="4">
-        <v>591.79999999999995</v>
-      </c>
-    </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="N37" t="s">
-        <v>156</v>
-      </c>
-      <c r="O37" s="2">
-        <v>42566</v>
-      </c>
-      <c r="P37" t="s">
-        <v>161</v>
-      </c>
-      <c r="Q37">
-        <v>2</v>
-      </c>
-      <c r="R37" t="s">
-        <v>166</v>
-      </c>
-      <c r="S37" s="4">
-        <v>15.256</v>
-      </c>
-      <c r="T37" s="4">
-        <v>569.89599999999996</v>
-      </c>
-    </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="N38" t="s">
-        <v>156</v>
-      </c>
-      <c r="O38" s="2">
-        <v>42566</v>
-      </c>
-      <c r="P38" t="s">
-        <v>162</v>
-      </c>
-      <c r="Q38">
-        <v>1</v>
-      </c>
-      <c r="R38" t="s">
-        <v>157</v>
-      </c>
-      <c r="S38" s="4">
-        <v>9.6509999999999998</v>
-      </c>
-      <c r="T38" s="4">
-        <v>507.07600000000002</v>
-      </c>
-    </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="N39" t="s">
-        <v>156</v>
-      </c>
-      <c r="O39" s="2">
-        <v>42566</v>
-      </c>
-      <c r="P39" t="s">
-        <v>162</v>
-      </c>
-      <c r="Q39">
-        <v>2</v>
-      </c>
-      <c r="R39" t="s">
-        <v>157</v>
-      </c>
-      <c r="S39" s="4">
-        <v>7.8860000000000001</v>
-      </c>
-      <c r="T39" s="4">
-        <v>492.93400000000003</v>
-      </c>
-    </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="N40" t="s">
-        <v>156</v>
-      </c>
-      <c r="O40" s="2">
-        <v>42566</v>
-      </c>
-      <c r="P40" t="s">
-        <v>162</v>
-      </c>
-      <c r="Q40">
-        <v>1</v>
-      </c>
-      <c r="R40" t="s">
-        <v>166</v>
-      </c>
-      <c r="S40" s="4">
-        <v>17.042000000000002</v>
-      </c>
-      <c r="T40" s="4">
-        <v>587.56500000000005</v>
-      </c>
-    </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="N41" t="s">
-        <v>156</v>
-      </c>
-      <c r="O41" s="2">
-        <v>42566</v>
-      </c>
-      <c r="P41" t="s">
-        <v>162</v>
-      </c>
-      <c r="Q41">
-        <v>2</v>
-      </c>
-      <c r="R41" t="s">
-        <v>166</v>
-      </c>
-      <c r="S41" s="4">
-        <v>17.109000000000002</v>
-      </c>
-      <c r="T41" s="4">
-        <v>585.19399999999996</v>
-      </c>
-    </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="N42" t="s">
-        <v>156</v>
-      </c>
-      <c r="O42" s="2">
-        <v>42566</v>
-      </c>
-      <c r="P42" t="s">
-        <v>163</v>
-      </c>
-      <c r="Q42">
-        <v>1</v>
-      </c>
-      <c r="R42" t="s">
-        <v>157</v>
-      </c>
-      <c r="S42" s="4">
-        <v>7.7930000000000001</v>
-      </c>
-      <c r="T42" s="4">
-        <v>552.98800000000006</v>
-      </c>
-    </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="N43" t="s">
-        <v>156</v>
-      </c>
-      <c r="O43" s="2">
-        <v>42566</v>
-      </c>
-      <c r="P43" t="s">
-        <v>163</v>
-      </c>
-      <c r="Q43">
-        <v>2</v>
-      </c>
-      <c r="R43" t="s">
-        <v>157</v>
-      </c>
-      <c r="S43" s="4">
-        <v>7.6559999999999997</v>
-      </c>
-      <c r="T43" s="4">
-        <v>688.06299999999999</v>
-      </c>
-    </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="N44" t="s">
-        <v>156</v>
-      </c>
-      <c r="O44" s="2">
-        <v>42566</v>
-      </c>
-      <c r="P44" t="s">
-        <v>163</v>
-      </c>
-      <c r="Q44">
-        <v>1</v>
-      </c>
-      <c r="R44" t="s">
-        <v>166</v>
-      </c>
-      <c r="S44" s="4">
-        <v>16.254000000000001</v>
-      </c>
-      <c r="T44" s="4">
-        <v>628.55600000000004</v>
-      </c>
-    </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="N45" t="s">
-        <v>156</v>
-      </c>
-      <c r="O45" s="2">
-        <v>42566</v>
-      </c>
-      <c r="P45" t="s">
-        <v>163</v>
-      </c>
-      <c r="Q45">
-        <v>2</v>
-      </c>
-      <c r="R45" t="s">
-        <v>166</v>
-      </c>
-      <c r="S45" s="4">
-        <v>16.297999999999998</v>
-      </c>
-      <c r="T45" s="4">
-        <v>629.78599999999994</v>
-      </c>
-    </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="N46" t="s">
-        <v>156</v>
-      </c>
-      <c r="O46" s="2">
-        <v>42567</v>
-      </c>
-      <c r="P46" t="s">
-        <v>164</v>
-      </c>
-      <c r="Q46">
-        <v>1</v>
-      </c>
-      <c r="R46" t="s">
-        <v>157</v>
-      </c>
-      <c r="S46" s="4">
-        <v>7.633</v>
-      </c>
-      <c r="T46" s="4">
-        <v>554.66700000000003</v>
-      </c>
-    </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="N47" t="s">
-        <v>156</v>
-      </c>
-      <c r="O47" s="2">
-        <v>42567</v>
-      </c>
-      <c r="P47" t="s">
-        <v>164</v>
-      </c>
-      <c r="Q47">
-        <v>2</v>
-      </c>
-      <c r="R47" t="s">
-        <v>157</v>
-      </c>
-      <c r="S47" s="4">
-        <v>7.6059999999999999</v>
-      </c>
-      <c r="T47" s="4">
-        <v>568.21400000000006</v>
-      </c>
-    </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="N48" t="s">
-        <v>156</v>
-      </c>
-      <c r="O48" s="2">
-        <v>42567</v>
-      </c>
-      <c r="P48" t="s">
-        <v>164</v>
-      </c>
-      <c r="Q48">
-        <v>1</v>
-      </c>
-      <c r="R48" t="s">
-        <v>166</v>
-      </c>
-      <c r="S48" s="4">
-        <v>18.655999999999999</v>
-      </c>
-      <c r="T48" s="4">
-        <v>677.79</v>
-      </c>
-    </row>
-    <row r="49" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N49" t="s">
-        <v>156</v>
-      </c>
-      <c r="O49" s="2">
-        <v>42567</v>
-      </c>
-      <c r="P49" t="s">
-        <v>164</v>
-      </c>
-      <c r="Q49">
-        <v>2</v>
-      </c>
-      <c r="R49" t="s">
-        <v>166</v>
-      </c>
-      <c r="S49" s="4">
-        <v>17.789000000000001</v>
-      </c>
-      <c r="T49" s="4">
-        <v>659.99900000000002</v>
-      </c>
-    </row>
-    <row r="50" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N50" t="s">
-        <v>154</v>
-      </c>
-      <c r="O50" s="2">
-        <v>42557</v>
-      </c>
-      <c r="P50" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="Q50">
-        <v>1</v>
-      </c>
-      <c r="R50" t="s">
-        <v>157</v>
-      </c>
-      <c r="S50" s="4">
-        <v>5.5469999999999997</v>
-      </c>
-      <c r="T50" s="4">
-        <v>332.04300000000001</v>
-      </c>
-    </row>
-    <row r="51" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N51" t="s">
-        <v>154</v>
-      </c>
-      <c r="O51" s="2">
-        <v>42557</v>
-      </c>
-      <c r="P51" t="s">
-        <v>159</v>
-      </c>
-      <c r="Q51">
-        <v>2</v>
-      </c>
-      <c r="R51" t="s">
-        <v>157</v>
-      </c>
-      <c r="S51" s="4">
-        <v>5.7629999999999999</v>
-      </c>
-      <c r="T51" s="4">
-        <v>325.755</v>
-      </c>
-    </row>
-    <row r="52" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N52" t="s">
-        <v>154</v>
-      </c>
-      <c r="O52" s="2">
-        <v>42557</v>
-      </c>
-      <c r="P52" t="s">
-        <v>159</v>
-      </c>
-      <c r="Q52">
-        <v>1</v>
-      </c>
-      <c r="R52" t="s">
-        <v>166</v>
-      </c>
-      <c r="S52" s="4">
-        <v>6.8280000000000003</v>
-      </c>
-      <c r="T52" s="4">
-        <v>339.75099999999998</v>
-      </c>
-    </row>
-    <row r="53" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N53" t="s">
-        <v>154</v>
-      </c>
-      <c r="O53" s="2">
-        <v>42557</v>
-      </c>
-      <c r="P53" t="s">
-        <v>159</v>
-      </c>
-      <c r="Q53">
-        <v>2</v>
-      </c>
-      <c r="R53" t="s">
-        <v>166</v>
-      </c>
-      <c r="S53" s="4">
-        <v>7.5380000000000003</v>
-      </c>
-      <c r="T53" s="4">
-        <v>360.15199999999999</v>
-      </c>
-    </row>
-    <row r="54" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N54" t="s">
-        <v>154</v>
-      </c>
-      <c r="O54" s="2">
-        <v>42557</v>
-      </c>
-      <c r="P54" t="s">
-        <v>160</v>
-      </c>
-      <c r="Q54">
-        <v>1</v>
-      </c>
-      <c r="R54" t="s">
-        <v>157</v>
-      </c>
-      <c r="S54" s="4">
-        <v>4.1760000000000002</v>
-      </c>
-      <c r="T54" s="4">
-        <v>368.88200000000001</v>
-      </c>
-    </row>
-    <row r="55" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N55" t="s">
-        <v>154</v>
-      </c>
-      <c r="O55" s="2">
-        <v>42557</v>
-      </c>
-      <c r="P55" t="s">
-        <v>160</v>
-      </c>
-      <c r="Q55">
-        <v>2</v>
-      </c>
-      <c r="R55" t="s">
-        <v>157</v>
-      </c>
-      <c r="S55" s="4">
-        <v>4.7190000000000003</v>
-      </c>
-      <c r="T55" s="4">
-        <v>352.87799999999999</v>
-      </c>
-    </row>
-    <row r="56" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N56" t="s">
-        <v>154</v>
-      </c>
-      <c r="O56" s="2">
-        <v>42557</v>
-      </c>
-      <c r="P56" t="s">
-        <v>160</v>
-      </c>
-      <c r="Q56">
-        <v>1</v>
-      </c>
-      <c r="R56" t="s">
-        <v>166</v>
-      </c>
-      <c r="S56" s="4">
-        <v>5.1509999999999998</v>
-      </c>
-      <c r="T56" s="4">
-        <v>388.601</v>
-      </c>
-    </row>
-    <row r="57" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N57" t="s">
-        <v>154</v>
-      </c>
-      <c r="O57" s="2">
-        <v>42557</v>
-      </c>
-      <c r="P57" t="s">
-        <v>160</v>
-      </c>
-      <c r="Q57">
-        <v>2</v>
-      </c>
-      <c r="R57" t="s">
-        <v>166</v>
-      </c>
-      <c r="S57" s="4">
-        <v>9.4600000000000009</v>
-      </c>
-      <c r="T57" s="4">
-        <v>425.73599999999999</v>
-      </c>
-    </row>
-    <row r="58" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N58" t="s">
-        <v>154</v>
-      </c>
-      <c r="O58" s="2">
-        <v>42557</v>
-      </c>
-      <c r="P58" t="s">
-        <v>161</v>
-      </c>
-      <c r="Q58">
-        <v>1</v>
-      </c>
-      <c r="R58" t="s">
-        <v>157</v>
-      </c>
-      <c r="S58" s="4">
-        <v>4.8780000000000001</v>
-      </c>
-      <c r="T58" s="4">
-        <v>337.63900000000001</v>
-      </c>
-    </row>
-    <row r="59" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N59" t="s">
-        <v>154</v>
-      </c>
-      <c r="O59" s="2">
-        <v>42557</v>
-      </c>
-      <c r="P59" t="s">
-        <v>161</v>
-      </c>
-      <c r="Q59">
-        <v>2</v>
-      </c>
-      <c r="R59" t="s">
-        <v>157</v>
-      </c>
-      <c r="S59" s="4">
-        <v>5.3170000000000002</v>
-      </c>
-      <c r="T59" s="4">
-        <v>339.92899999999997</v>
-      </c>
-    </row>
-    <row r="60" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N60" t="s">
-        <v>154</v>
-      </c>
-      <c r="O60" s="2">
-        <v>42557</v>
-      </c>
-      <c r="P60" t="s">
-        <v>161</v>
-      </c>
-      <c r="Q60">
-        <v>1</v>
-      </c>
-      <c r="R60" t="s">
-        <v>166</v>
-      </c>
-      <c r="S60" s="4">
-        <v>4.33</v>
-      </c>
-      <c r="T60" s="4">
-        <v>334.93299999999999</v>
-      </c>
-    </row>
-    <row r="61" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N61" t="s">
-        <v>154</v>
-      </c>
-      <c r="O61" s="2">
-        <v>42557</v>
-      </c>
-      <c r="P61" t="s">
-        <v>161</v>
-      </c>
-      <c r="Q61">
-        <v>2</v>
-      </c>
-      <c r="R61" t="s">
-        <v>166</v>
-      </c>
-      <c r="S61" s="4">
-        <v>8.0350000000000001</v>
-      </c>
-      <c r="T61" s="4">
-        <v>482.505</v>
-      </c>
-    </row>
-    <row r="62" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N62" t="s">
-        <v>154</v>
-      </c>
-      <c r="O62" s="2">
-        <v>42557</v>
-      </c>
-      <c r="P62" t="s">
-        <v>162</v>
-      </c>
-      <c r="Q62">
-        <v>1</v>
-      </c>
-      <c r="R62" t="s">
-        <v>157</v>
-      </c>
-      <c r="S62" s="4">
-        <v>6.569</v>
-      </c>
-      <c r="T62" s="4">
-        <v>278.12400000000002</v>
-      </c>
-    </row>
-    <row r="63" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N63" t="s">
-        <v>154</v>
-      </c>
-      <c r="O63" s="2">
-        <v>42557</v>
-      </c>
-      <c r="P63" t="s">
-        <v>162</v>
-      </c>
-      <c r="Q63">
-        <v>2</v>
-      </c>
-      <c r="R63" t="s">
-        <v>157</v>
-      </c>
-      <c r="S63" s="4">
-        <v>6.1580000000000004</v>
-      </c>
-      <c r="T63" s="4">
-        <v>265.10700000000003</v>
-      </c>
-    </row>
-    <row r="64" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N64" t="s">
-        <v>154</v>
-      </c>
-      <c r="O64" s="2">
-        <v>42557</v>
-      </c>
-      <c r="P64" t="s">
-        <v>162</v>
-      </c>
-      <c r="Q64">
-        <v>1</v>
-      </c>
-      <c r="R64" t="s">
-        <v>166</v>
-      </c>
-      <c r="S64" s="4">
-        <v>5.532</v>
-      </c>
-      <c r="T64" s="4">
-        <v>253.726</v>
-      </c>
-    </row>
-    <row r="65" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N65" t="s">
-        <v>154</v>
-      </c>
-      <c r="O65" s="2">
-        <v>42557</v>
-      </c>
-      <c r="P65" t="s">
-        <v>162</v>
-      </c>
-      <c r="Q65">
-        <v>2</v>
-      </c>
-      <c r="R65" t="s">
-        <v>166</v>
-      </c>
-      <c r="S65" s="4">
-        <v>3.9940000000000002</v>
-      </c>
-      <c r="T65" s="4">
-        <v>240.26300000000001</v>
-      </c>
-    </row>
-    <row r="66" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N66" t="s">
-        <v>154</v>
-      </c>
-      <c r="O66" s="2">
-        <v>42557</v>
-      </c>
-      <c r="P66" t="s">
-        <v>163</v>
-      </c>
-      <c r="Q66">
-        <v>1</v>
-      </c>
-      <c r="R66" t="s">
-        <v>157</v>
-      </c>
-      <c r="S66" s="4">
-        <v>5.3659999999999997</v>
-      </c>
-      <c r="T66" s="4">
-        <v>285.358</v>
-      </c>
-    </row>
-    <row r="67" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N67" t="s">
-        <v>154</v>
-      </c>
-      <c r="O67" s="2">
-        <v>42557</v>
-      </c>
-      <c r="P67" t="s">
-        <v>163</v>
-      </c>
-      <c r="Q67">
-        <v>2</v>
-      </c>
-      <c r="R67" t="s">
-        <v>157</v>
-      </c>
-      <c r="S67" s="4">
-        <v>4.165</v>
-      </c>
-      <c r="T67" s="4">
-        <v>284.79700000000003</v>
-      </c>
-    </row>
-    <row r="68" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N68" t="s">
-        <v>154</v>
-      </c>
-      <c r="O68" s="2">
-        <v>42557</v>
-      </c>
-      <c r="P68" t="s">
-        <v>163</v>
-      </c>
-      <c r="Q68">
-        <v>1</v>
-      </c>
-      <c r="R68" t="s">
-        <v>166</v>
-      </c>
-      <c r="S68" s="4">
-        <v>7.1989999999999998</v>
-      </c>
-      <c r="T68" s="4">
-        <v>451.375</v>
-      </c>
-    </row>
-    <row r="69" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N69" t="s">
-        <v>154</v>
-      </c>
-      <c r="O69" s="2">
-        <v>42557</v>
-      </c>
-      <c r="P69" t="s">
-        <v>163</v>
-      </c>
-      <c r="Q69">
-        <v>2</v>
-      </c>
-      <c r="R69" t="s">
-        <v>166</v>
-      </c>
-      <c r="S69" s="4">
-        <v>9.0419999999999998</v>
-      </c>
-      <c r="T69" s="4">
-        <v>556.39099999999996</v>
-      </c>
-    </row>
-    <row r="70" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N70" t="s">
-        <v>154</v>
-      </c>
-      <c r="O70" s="2">
-        <v>42558</v>
-      </c>
-      <c r="P70" t="s">
-        <v>164</v>
-      </c>
-      <c r="Q70">
-        <v>1</v>
-      </c>
-      <c r="R70" t="s">
-        <v>157</v>
-      </c>
-      <c r="S70" s="4">
-        <v>7.8339999999999996</v>
-      </c>
-      <c r="T70" s="4">
-        <v>386.85899999999998</v>
-      </c>
-    </row>
-    <row r="71" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N71" t="s">
-        <v>154</v>
-      </c>
-      <c r="O71" s="2">
-        <v>42558</v>
-      </c>
-      <c r="P71" t="s">
-        <v>164</v>
-      </c>
-      <c r="Q71">
-        <v>2</v>
-      </c>
-      <c r="R71" t="s">
-        <v>157</v>
-      </c>
-      <c r="S71" s="4">
-        <v>5.6539999999999999</v>
-      </c>
-      <c r="T71" s="4">
-        <v>356.94</v>
-      </c>
-    </row>
-    <row r="72" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N72" t="s">
-        <v>154</v>
-      </c>
-      <c r="O72" s="2">
-        <v>42558</v>
-      </c>
-      <c r="P72" t="s">
-        <v>164</v>
-      </c>
-      <c r="Q72">
-        <v>1</v>
-      </c>
-      <c r="R72" t="s">
-        <v>166</v>
-      </c>
-      <c r="S72" s="4">
-        <v>6.7869999999999999</v>
-      </c>
-      <c r="T72" s="4">
-        <v>373.64100000000002</v>
-      </c>
-    </row>
-    <row r="73" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N73" t="s">
-        <v>154</v>
-      </c>
-      <c r="O73" s="2">
-        <v>42558</v>
-      </c>
-      <c r="P73" t="s">
-        <v>164</v>
-      </c>
-      <c r="Q73">
-        <v>2</v>
-      </c>
-      <c r="R73" t="s">
-        <v>166</v>
-      </c>
-      <c r="S73" s="4">
-        <v>6.4450000000000003</v>
-      </c>
-      <c r="T73" s="4">
-        <v>377.32400000000001</v>
-      </c>
-    </row>
-    <row r="74" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N74" t="s">
-        <v>154</v>
-      </c>
-      <c r="O74" s="2">
-        <v>42558</v>
-      </c>
-      <c r="P74" t="s">
-        <v>159</v>
-      </c>
-      <c r="Q74">
-        <v>1</v>
-      </c>
-      <c r="R74" t="s">
-        <v>157</v>
-      </c>
-      <c r="S74" s="4">
-        <v>6.3559999999999999</v>
-      </c>
-      <c r="T74" s="4">
-        <v>324.38900000000001</v>
-      </c>
-    </row>
-    <row r="75" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N75" t="s">
-        <v>154</v>
-      </c>
-      <c r="O75" s="2">
-        <v>42558</v>
-      </c>
-      <c r="P75" t="s">
-        <v>159</v>
-      </c>
-      <c r="Q75">
-        <v>2</v>
-      </c>
-      <c r="R75" t="s">
-        <v>157</v>
-      </c>
-      <c r="S75" s="4">
-        <v>7.3369999999999997</v>
-      </c>
-      <c r="T75" s="4">
-        <v>339.07900000000001</v>
-      </c>
-    </row>
-    <row r="76" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N76" t="s">
-        <v>154</v>
-      </c>
-      <c r="O76" s="2">
-        <v>42558</v>
-      </c>
-      <c r="P76" t="s">
-        <v>159</v>
-      </c>
-      <c r="Q76">
-        <v>1</v>
-      </c>
-      <c r="R76" t="s">
-        <v>166</v>
-      </c>
-      <c r="S76" s="4">
-        <v>7.1769999999999996</v>
-      </c>
-      <c r="T76" s="4">
-        <v>307.14299999999997</v>
-      </c>
-    </row>
-    <row r="77" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N77" t="s">
-        <v>154</v>
-      </c>
-      <c r="O77" s="2">
-        <v>42558</v>
-      </c>
-      <c r="P77" t="s">
-        <v>159</v>
-      </c>
-      <c r="Q77">
-        <v>2</v>
-      </c>
-      <c r="R77" t="s">
-        <v>166</v>
-      </c>
-      <c r="S77" s="4">
-        <v>6.8490000000000002</v>
-      </c>
-      <c r="T77" s="4">
-        <v>302.55700000000002</v>
-      </c>
-    </row>
-    <row r="78" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N78" t="s">
-        <v>154</v>
-      </c>
-      <c r="O78" s="2">
-        <v>42558</v>
-      </c>
-      <c r="P78" t="s">
-        <v>160</v>
-      </c>
-      <c r="Q78">
-        <v>1</v>
-      </c>
-      <c r="R78" t="s">
-        <v>157</v>
-      </c>
-      <c r="S78" s="4">
-        <v>5.6970000000000001</v>
-      </c>
-      <c r="T78" s="4">
-        <v>287.06700000000001</v>
-      </c>
-    </row>
-    <row r="79" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N79" t="s">
-        <v>154</v>
-      </c>
-      <c r="O79" s="2">
-        <v>42558</v>
-      </c>
-      <c r="P79" t="s">
-        <v>160</v>
-      </c>
-      <c r="Q79">
-        <v>2</v>
-      </c>
-      <c r="R79" t="s">
-        <v>157</v>
-      </c>
-      <c r="S79" s="4">
-        <v>4.5780000000000003</v>
-      </c>
-      <c r="T79" s="4">
-        <v>273.666</v>
-      </c>
-    </row>
-    <row r="80" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N80" t="s">
-        <v>154</v>
-      </c>
-      <c r="O80" s="2">
-        <v>42558</v>
-      </c>
-      <c r="P80" t="s">
-        <v>160</v>
-      </c>
-      <c r="Q80">
-        <v>1</v>
-      </c>
-      <c r="R80" t="s">
-        <v>166</v>
-      </c>
-      <c r="S80" s="4">
-        <v>5.1459999999999999</v>
-      </c>
-      <c r="T80" s="4">
-        <v>293.57600000000002</v>
-      </c>
-    </row>
-    <row r="81" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N81" t="s">
-        <v>154</v>
-      </c>
-      <c r="O81" s="2">
-        <v>42558</v>
-      </c>
-      <c r="P81" t="s">
-        <v>160</v>
-      </c>
-      <c r="Q81">
-        <v>2</v>
-      </c>
-      <c r="R81" t="s">
-        <v>166</v>
-      </c>
-      <c r="S81" s="4">
-        <v>9.766</v>
-      </c>
-      <c r="T81" s="4">
-        <v>372.66500000000002</v>
-      </c>
-    </row>
-    <row r="82" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N82" t="s">
-        <v>154</v>
-      </c>
-      <c r="O82" s="2">
-        <v>42558</v>
-      </c>
-      <c r="P82" t="s">
-        <v>161</v>
-      </c>
-      <c r="Q82">
-        <v>1</v>
-      </c>
-      <c r="R82" t="s">
-        <v>157</v>
-      </c>
-      <c r="S82" s="4">
-        <v>6.1669999999999998</v>
-      </c>
-      <c r="T82" s="4">
-        <v>248.82</v>
-      </c>
-    </row>
-    <row r="83" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N83" t="s">
-        <v>154</v>
-      </c>
-      <c r="O83" s="2">
-        <v>42558</v>
-      </c>
-      <c r="P83" t="s">
-        <v>161</v>
-      </c>
-      <c r="Q83">
-        <v>2</v>
-      </c>
-      <c r="R83" t="s">
-        <v>157</v>
-      </c>
-      <c r="S83" s="4">
-        <v>5.048</v>
-      </c>
-      <c r="T83" s="4">
-        <v>251.92</v>
-      </c>
-    </row>
-    <row r="84" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N84" t="s">
-        <v>154</v>
-      </c>
-      <c r="O84" s="2">
-        <v>42558</v>
-      </c>
-      <c r="P84" t="s">
-        <v>161</v>
-      </c>
-      <c r="Q84">
-        <v>1</v>
-      </c>
-      <c r="R84" t="s">
-        <v>166</v>
-      </c>
-      <c r="S84" s="4">
-        <v>6.0670000000000002</v>
-      </c>
-      <c r="T84" s="4">
-        <v>285.42200000000003</v>
-      </c>
-    </row>
-    <row r="85" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N85" t="s">
-        <v>154</v>
-      </c>
-      <c r="O85" s="2">
-        <v>42558</v>
-      </c>
-      <c r="P85" t="s">
-        <v>161</v>
-      </c>
-      <c r="Q85">
-        <v>2</v>
-      </c>
-      <c r="R85" t="s">
-        <v>166</v>
-      </c>
-      <c r="S85" s="4">
-        <v>4.6420000000000003</v>
-      </c>
-      <c r="T85" s="4">
-        <v>265.42</v>
-      </c>
-    </row>
-    <row r="86" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N86" t="s">
-        <v>154</v>
-      </c>
-      <c r="O86" s="2">
-        <v>42558</v>
-      </c>
-      <c r="P86" t="s">
-        <v>162</v>
-      </c>
-      <c r="Q86">
-        <v>1</v>
-      </c>
-      <c r="R86" t="s">
-        <v>157</v>
-      </c>
-      <c r="S86" s="4">
-        <v>2.0379999999999998</v>
-      </c>
-      <c r="T86" s="4">
-        <v>237.55699999999999</v>
-      </c>
-    </row>
-    <row r="87" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N87" t="s">
-        <v>154</v>
-      </c>
-      <c r="O87" s="2">
-        <v>42558</v>
-      </c>
-      <c r="P87" t="s">
-        <v>162</v>
-      </c>
-      <c r="Q87">
-        <v>2</v>
-      </c>
-      <c r="R87" t="s">
-        <v>157</v>
-      </c>
-      <c r="S87" s="4">
-        <v>1.9350000000000001</v>
-      </c>
-      <c r="T87" s="4">
-        <v>220.55199999999999</v>
-      </c>
-    </row>
-    <row r="88" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N88" t="s">
-        <v>154</v>
-      </c>
-      <c r="O88" s="2">
-        <v>42558</v>
-      </c>
-      <c r="P88" t="s">
-        <v>162</v>
-      </c>
-      <c r="Q88">
-        <v>1</v>
-      </c>
-      <c r="R88" t="s">
-        <v>166</v>
-      </c>
-      <c r="S88" s="4">
-        <v>5.3890000000000002</v>
-      </c>
-      <c r="T88" s="4">
-        <v>253.61600000000001</v>
-      </c>
-    </row>
-    <row r="89" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N89" t="s">
-        <v>154</v>
-      </c>
-      <c r="O89" s="2">
-        <v>42558</v>
-      </c>
-      <c r="P89" t="s">
-        <v>162</v>
-      </c>
-      <c r="Q89">
-        <v>2</v>
-      </c>
-      <c r="R89" t="s">
-        <v>166</v>
-      </c>
-      <c r="S89" s="4">
-        <v>4.3</v>
-      </c>
-      <c r="T89" s="4">
-        <v>243.88</v>
-      </c>
-    </row>
-    <row r="90" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N90" t="s">
-        <v>154</v>
-      </c>
-      <c r="O90" s="2">
-        <v>42558</v>
-      </c>
-      <c r="P90" t="s">
-        <v>163</v>
-      </c>
-      <c r="Q90">
-        <v>1</v>
-      </c>
-      <c r="R90" t="s">
-        <v>157</v>
-      </c>
-      <c r="S90" s="4">
-        <v>7.02</v>
-      </c>
-      <c r="T90" s="4">
-        <v>316.70800000000003</v>
-      </c>
-    </row>
-    <row r="91" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N91" t="s">
-        <v>154</v>
-      </c>
-      <c r="O91" s="2">
-        <v>42558</v>
-      </c>
-      <c r="P91" t="s">
-        <v>163</v>
-      </c>
-      <c r="Q91">
-        <v>2</v>
-      </c>
-      <c r="R91" t="s">
-        <v>157</v>
-      </c>
-      <c r="S91" s="4">
-        <v>6.8929999999999998</v>
-      </c>
-      <c r="T91" s="4">
-        <v>321.50099999999998</v>
-      </c>
-    </row>
-    <row r="92" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N92" t="s">
-        <v>154</v>
-      </c>
-      <c r="O92" s="2">
-        <v>42558</v>
-      </c>
-      <c r="P92" t="s">
-        <v>163</v>
-      </c>
-      <c r="Q92">
-        <v>1</v>
-      </c>
-      <c r="R92" t="s">
-        <v>166</v>
-      </c>
-      <c r="S92" s="4">
-        <v>5.8040000000000003</v>
-      </c>
-      <c r="T92" s="4">
-        <v>390.89600000000002</v>
-      </c>
-    </row>
-    <row r="93" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N93" t="s">
-        <v>154</v>
-      </c>
-      <c r="O93" s="2">
-        <v>42558</v>
-      </c>
-      <c r="P93" t="s">
-        <v>163</v>
-      </c>
-      <c r="Q93">
-        <v>2</v>
-      </c>
-      <c r="R93" t="s">
-        <v>166</v>
-      </c>
-      <c r="S93" s="4">
-        <v>6.2949999999999999</v>
-      </c>
-      <c r="T93" s="4">
-        <v>322.49200000000002</v>
-      </c>
-    </row>
-    <row r="94" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N94" t="s">
-        <v>154</v>
-      </c>
-      <c r="O94" s="2">
-        <v>42560</v>
-      </c>
-      <c r="P94" t="s">
-        <v>164</v>
-      </c>
-      <c r="Q94">
-        <v>1</v>
-      </c>
-      <c r="R94" t="s">
-        <v>157</v>
-      </c>
-      <c r="S94" s="4">
-        <v>5.3319999999999999</v>
-      </c>
-      <c r="T94" s="4">
-        <v>319.45</v>
-      </c>
-    </row>
-    <row r="95" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N95" t="s">
-        <v>154</v>
-      </c>
-      <c r="O95" s="2">
-        <v>42560</v>
-      </c>
-      <c r="P95" t="s">
-        <v>164</v>
-      </c>
-      <c r="Q95">
-        <v>2</v>
-      </c>
-      <c r="R95" t="s">
-        <v>157</v>
-      </c>
-      <c r="S95" s="4">
-        <v>4.3730000000000002</v>
-      </c>
-      <c r="T95" s="4">
-        <v>316.45299999999997</v>
-      </c>
-    </row>
-    <row r="96" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N96" t="s">
-        <v>154</v>
-      </c>
-      <c r="O96" s="2">
-        <v>42560</v>
-      </c>
-      <c r="P96" t="s">
-        <v>164</v>
-      </c>
-      <c r="Q96">
-        <v>1</v>
-      </c>
-      <c r="R96" t="s">
-        <v>166</v>
-      </c>
-      <c r="S96" s="4">
-        <v>6.4710000000000001</v>
-      </c>
-      <c r="T96" s="4">
-        <v>343.43700000000001</v>
-      </c>
-    </row>
-    <row r="97" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N97" t="s">
-        <v>154</v>
-      </c>
-      <c r="O97" s="2">
-        <v>42560</v>
-      </c>
-      <c r="P97" t="s">
-        <v>164</v>
-      </c>
-      <c r="Q97">
-        <v>2</v>
-      </c>
-      <c r="R97" t="s">
-        <v>166</v>
-      </c>
-      <c r="S97" s="4">
-        <v>7.407</v>
-      </c>
-      <c r="T97" s="4">
-        <v>340.17099999999999</v>
-      </c>
-    </row>
-    <row r="98" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N98" t="s">
-        <v>155</v>
-      </c>
-      <c r="O98" s="2">
-        <v>42559</v>
-      </c>
-      <c r="P98" t="s">
-        <v>159</v>
-      </c>
-      <c r="Q98">
-        <v>1</v>
-      </c>
-      <c r="R98" t="s">
-        <v>157</v>
-      </c>
-      <c r="S98" s="4">
-        <v>15.08</v>
-      </c>
-      <c r="T98" s="4">
-        <v>536.00199999999995</v>
-      </c>
-    </row>
-    <row r="99" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N99" t="s">
-        <v>155</v>
-      </c>
-      <c r="O99" s="2">
-        <v>42559</v>
-      </c>
-      <c r="P99" t="s">
-        <v>159</v>
-      </c>
-      <c r="Q99">
-        <v>2</v>
-      </c>
-      <c r="R99" t="s">
-        <v>157</v>
-      </c>
-      <c r="S99" s="4">
-        <v>13.87</v>
-      </c>
-      <c r="T99" s="4">
-        <v>567.15800000000002</v>
-      </c>
-    </row>
-    <row r="100" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N100" t="s">
-        <v>155</v>
-      </c>
-      <c r="O100" s="2">
-        <v>42559</v>
-      </c>
-      <c r="P100" t="s">
-        <v>159</v>
-      </c>
-      <c r="Q100">
-        <v>1</v>
-      </c>
-      <c r="R100" t="s">
-        <v>166</v>
-      </c>
-      <c r="S100" s="4">
-        <v>20.257999999999999</v>
-      </c>
-      <c r="T100" s="4">
-        <v>604.91899999999998</v>
-      </c>
-    </row>
-    <row r="101" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N101" t="s">
-        <v>155</v>
-      </c>
-      <c r="O101" s="2">
-        <v>42559</v>
-      </c>
-      <c r="P101" t="s">
-        <v>159</v>
-      </c>
-      <c r="Q101">
-        <v>2</v>
-      </c>
-      <c r="R101" t="s">
-        <v>166</v>
-      </c>
-      <c r="S101" s="4">
-        <v>18.018999999999998</v>
-      </c>
-      <c r="T101" s="4">
-        <v>598.053</v>
-      </c>
-    </row>
-    <row r="102" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N102" t="s">
-        <v>155</v>
-      </c>
-      <c r="O102" s="2">
-        <v>42559</v>
-      </c>
-      <c r="P102" t="s">
-        <v>160</v>
-      </c>
-      <c r="Q102">
-        <v>1</v>
-      </c>
-      <c r="R102" t="s">
-        <v>157</v>
-      </c>
-      <c r="S102" s="4">
-        <v>14.637</v>
-      </c>
-      <c r="T102" s="4">
-        <v>537.81899999999996</v>
-      </c>
-    </row>
-    <row r="103" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N103" t="s">
-        <v>155</v>
-      </c>
-      <c r="O103" s="2">
-        <v>42559</v>
-      </c>
-      <c r="P103" t="s">
-        <v>160</v>
-      </c>
-      <c r="Q103">
-        <v>2</v>
-      </c>
-      <c r="R103" t="s">
-        <v>157</v>
-      </c>
-      <c r="S103" s="4">
-        <v>11.571</v>
-      </c>
-      <c r="T103" s="4">
-        <v>565.33500000000004</v>
-      </c>
-    </row>
-    <row r="104" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N104" t="s">
-        <v>155</v>
-      </c>
-      <c r="O104" s="2">
-        <v>42559</v>
-      </c>
-      <c r="P104" t="s">
-        <v>160</v>
-      </c>
-      <c r="Q104">
-        <v>1</v>
-      </c>
-      <c r="R104" t="s">
-        <v>166</v>
-      </c>
-      <c r="S104" s="4">
-        <v>26.324999999999999</v>
-      </c>
-      <c r="T104" s="4">
-        <v>700.13800000000003</v>
-      </c>
-    </row>
-    <row r="105" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N105" t="s">
-        <v>155</v>
-      </c>
-      <c r="O105" s="2">
-        <v>42559</v>
-      </c>
-      <c r="P105" t="s">
-        <v>160</v>
-      </c>
-      <c r="Q105">
-        <v>2</v>
-      </c>
-      <c r="R105" t="s">
-        <v>166</v>
-      </c>
-      <c r="S105" s="4">
-        <v>27.606000000000002</v>
-      </c>
-      <c r="T105" s="4">
-        <v>713.92899999999997</v>
-      </c>
-    </row>
-    <row r="106" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N106" t="s">
-        <v>155</v>
-      </c>
-      <c r="O106" s="2">
-        <v>42559</v>
-      </c>
-      <c r="P106" t="s">
-        <v>161</v>
-      </c>
-      <c r="Q106">
-        <v>1</v>
-      </c>
-      <c r="R106" t="s">
-        <v>157</v>
-      </c>
-      <c r="S106" s="4">
-        <v>14.045999999999999</v>
-      </c>
-      <c r="T106" s="4">
-        <v>620.41800000000001</v>
-      </c>
-    </row>
-    <row r="107" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N107" t="s">
-        <v>155</v>
-      </c>
-      <c r="O107" s="2">
-        <v>42559</v>
-      </c>
-      <c r="P107" t="s">
-        <v>161</v>
-      </c>
-      <c r="Q107">
-        <v>2</v>
-      </c>
-      <c r="R107" t="s">
-        <v>157</v>
-      </c>
-      <c r="S107" s="4">
-        <v>14.625</v>
-      </c>
-      <c r="T107" s="4">
-        <v>565.42100000000005</v>
-      </c>
-    </row>
-    <row r="108" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N108" t="s">
-        <v>155</v>
-      </c>
-      <c r="O108" s="2">
-        <v>42559</v>
-      </c>
-      <c r="P108" t="s">
-        <v>161</v>
-      </c>
-      <c r="Q108">
-        <v>1</v>
-      </c>
-      <c r="R108" t="s">
-        <v>166</v>
-      </c>
-      <c r="S108" s="4">
-        <v>29.247</v>
-      </c>
-      <c r="T108" s="4">
-        <v>720.71799999999996</v>
-      </c>
-    </row>
-    <row r="109" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N109" t="s">
-        <v>155</v>
-      </c>
-      <c r="O109" s="2">
-        <v>42559</v>
-      </c>
-      <c r="P109" t="s">
-        <v>161</v>
-      </c>
-      <c r="Q109">
-        <v>2</v>
-      </c>
-      <c r="R109" t="s">
-        <v>166</v>
-      </c>
-      <c r="S109" s="4">
-        <v>31.957999999999998</v>
-      </c>
-      <c r="T109" s="4">
-        <v>736.13400000000001</v>
-      </c>
-    </row>
-    <row r="110" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N110" t="s">
-        <v>155</v>
-      </c>
-      <c r="O110" s="2">
-        <v>42559</v>
-      </c>
-      <c r="P110" t="s">
-        <v>162</v>
-      </c>
-      <c r="Q110">
-        <v>1</v>
-      </c>
-      <c r="R110" t="s">
-        <v>157</v>
-      </c>
-      <c r="S110" s="4">
-        <v>14.614000000000001</v>
-      </c>
-      <c r="T110" s="4">
-        <v>614.13499999999999</v>
-      </c>
-    </row>
-    <row r="111" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N111" t="s">
-        <v>155</v>
-      </c>
-      <c r="O111" s="2">
-        <v>42559</v>
-      </c>
-      <c r="P111" t="s">
-        <v>162</v>
-      </c>
-      <c r="Q111">
-        <v>2</v>
-      </c>
-      <c r="R111" t="s">
-        <v>157</v>
-      </c>
-      <c r="S111" s="4">
-        <v>16.498000000000001</v>
-      </c>
-      <c r="T111" s="4">
-        <v>598.73599999999999</v>
-      </c>
-    </row>
-    <row r="112" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N112" t="s">
-        <v>155</v>
-      </c>
-      <c r="O112" s="2">
-        <v>42559</v>
-      </c>
-      <c r="P112" t="s">
-        <v>162</v>
-      </c>
-      <c r="Q112">
-        <v>1</v>
-      </c>
-      <c r="R112" t="s">
-        <v>166</v>
-      </c>
-      <c r="S112" s="4">
-        <v>28.058</v>
-      </c>
-      <c r="T112" s="4">
-        <v>671.10199999999998</v>
-      </c>
-    </row>
-    <row r="113" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N113" t="s">
-        <v>155</v>
-      </c>
-      <c r="O113" s="2">
-        <v>42559</v>
-      </c>
-      <c r="P113" t="s">
-        <v>162</v>
-      </c>
-      <c r="Q113">
-        <v>2</v>
-      </c>
-      <c r="R113" t="s">
-        <v>166</v>
-      </c>
-      <c r="S113" s="4">
-        <v>18.004000000000001</v>
-      </c>
-      <c r="T113" s="4">
-        <v>612.46100000000001</v>
-      </c>
-    </row>
-    <row r="114" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N114" t="s">
-        <v>155</v>
-      </c>
-      <c r="O114" s="2">
-        <v>42559</v>
-      </c>
-      <c r="P114" t="s">
-        <v>163</v>
-      </c>
-      <c r="Q114">
-        <v>1</v>
-      </c>
-      <c r="R114" t="s">
-        <v>157</v>
-      </c>
-      <c r="S114" s="4">
-        <v>15.177</v>
-      </c>
-      <c r="T114" s="4">
-        <v>553.31399999999996</v>
-      </c>
-    </row>
-    <row r="115" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N115" t="s">
-        <v>155</v>
-      </c>
-      <c r="O115" s="2">
-        <v>42559</v>
-      </c>
-      <c r="P115" t="s">
-        <v>163</v>
-      </c>
-      <c r="Q115">
-        <v>2</v>
-      </c>
-      <c r="R115" t="s">
-        <v>157</v>
-      </c>
-      <c r="S115" s="4">
-        <v>15.803000000000001</v>
-      </c>
-      <c r="T115" s="4">
-        <v>554.88</v>
-      </c>
-    </row>
-    <row r="116" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N116" t="s">
-        <v>155</v>
-      </c>
-      <c r="O116" s="2">
-        <v>42559</v>
-      </c>
-      <c r="P116" t="s">
-        <v>163</v>
-      </c>
-      <c r="Q116">
-        <v>1</v>
-      </c>
-      <c r="R116" t="s">
-        <v>166</v>
-      </c>
-      <c r="S116" s="4">
-        <v>20.317</v>
-      </c>
-      <c r="T116" s="4">
-        <v>649.93200000000002</v>
-      </c>
-    </row>
-    <row r="117" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N117" t="s">
-        <v>155</v>
-      </c>
-      <c r="O117" s="2">
-        <v>42559</v>
-      </c>
-      <c r="P117" t="s">
-        <v>163</v>
-      </c>
-      <c r="Q117">
-        <v>2</v>
-      </c>
-      <c r="R117" t="s">
-        <v>166</v>
-      </c>
-      <c r="S117" s="4">
-        <v>16.384</v>
-      </c>
-      <c r="T117" s="4">
-        <v>591.26599999999996</v>
-      </c>
-    </row>
-    <row r="118" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N118" t="s">
-        <v>155</v>
-      </c>
-      <c r="O118" s="2">
-        <v>42560</v>
-      </c>
-      <c r="P118" t="s">
-        <v>164</v>
-      </c>
-      <c r="Q118">
-        <v>1</v>
-      </c>
-      <c r="R118" t="s">
-        <v>157</v>
-      </c>
-      <c r="S118" s="4">
-        <v>16.695</v>
-      </c>
-      <c r="T118" s="4">
-        <v>580.23800000000006</v>
-      </c>
-    </row>
-    <row r="119" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N119" t="s">
-        <v>155</v>
-      </c>
-      <c r="O119" s="2">
-        <v>42560</v>
-      </c>
-      <c r="P119" t="s">
-        <v>164</v>
-      </c>
-      <c r="Q119">
-        <v>2</v>
-      </c>
-      <c r="R119" t="s">
-        <v>157</v>
-      </c>
-      <c r="S119" s="4">
-        <v>13.911</v>
-      </c>
-      <c r="T119" s="4">
-        <v>600.97900000000004</v>
-      </c>
-    </row>
-    <row r="120" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N120" t="s">
-        <v>155</v>
-      </c>
-      <c r="O120" s="2">
-        <v>42560</v>
-      </c>
-      <c r="P120" t="s">
-        <v>164</v>
-      </c>
-      <c r="Q120">
-        <v>1</v>
-      </c>
-      <c r="R120" t="s">
-        <v>166</v>
-      </c>
-      <c r="S120" s="4">
-        <v>15.099</v>
-      </c>
-      <c r="T120" s="4">
-        <v>623.61900000000003</v>
-      </c>
-    </row>
-    <row r="121" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N121" t="s">
-        <v>155</v>
-      </c>
-      <c r="O121" s="2">
-        <v>42560</v>
-      </c>
-      <c r="P121" t="s">
-        <v>164</v>
-      </c>
-      <c r="Q121">
-        <v>2</v>
-      </c>
-      <c r="R121" t="s">
-        <v>166</v>
-      </c>
-      <c r="S121" s="4">
-        <v>23.844000000000001</v>
-      </c>
-      <c r="T121" s="4">
-        <v>702.11300000000006</v>
-      </c>
-    </row>
-    <row r="122" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N122" t="s">
-        <v>155</v>
-      </c>
-      <c r="O122" s="2">
-        <v>42560</v>
-      </c>
-      <c r="P122" t="s">
-        <v>159</v>
-      </c>
-      <c r="Q122">
-        <v>1</v>
-      </c>
-      <c r="R122" t="s">
-        <v>157</v>
-      </c>
-      <c r="S122" s="4">
-        <v>17.125</v>
-      </c>
-      <c r="T122" s="4">
-        <v>599.726</v>
-      </c>
-    </row>
-    <row r="123" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N123" t="s">
-        <v>155</v>
-      </c>
-      <c r="O123" s="2">
-        <v>42560</v>
-      </c>
-      <c r="P123" t="s">
-        <v>159</v>
-      </c>
-      <c r="Q123">
-        <v>2</v>
-      </c>
-      <c r="R123" t="s">
-        <v>157</v>
-      </c>
-      <c r="S123" s="4">
-        <v>15.25</v>
-      </c>
-      <c r="T123" s="4">
-        <v>552.74599999999998</v>
-      </c>
-    </row>
-    <row r="124" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N124" t="s">
-        <v>155</v>
-      </c>
-      <c r="O124" s="2">
-        <v>42560</v>
-      </c>
-      <c r="P124" t="s">
-        <v>159</v>
-      </c>
-      <c r="Q124">
-        <v>1</v>
-      </c>
-      <c r="R124" t="s">
-        <v>166</v>
-      </c>
-      <c r="S124" s="4">
-        <v>16.585999999999999</v>
-      </c>
-      <c r="T124" s="4">
-        <v>603.85</v>
-      </c>
-    </row>
-    <row r="125" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N125" t="s">
-        <v>155</v>
-      </c>
-      <c r="O125" s="2">
-        <v>42560</v>
-      </c>
-      <c r="P125" t="s">
-        <v>159</v>
-      </c>
-      <c r="Q125">
-        <v>2</v>
-      </c>
-      <c r="R125" t="s">
-        <v>166</v>
-      </c>
-      <c r="S125" s="4">
-        <v>18.437999999999999</v>
-      </c>
-      <c r="T125" s="4">
-        <v>607.41200000000003</v>
-      </c>
-    </row>
-    <row r="126" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N126" t="s">
-        <v>155</v>
-      </c>
-      <c r="O126" s="2">
-        <v>42560</v>
-      </c>
-      <c r="P126" t="s">
-        <v>160</v>
-      </c>
-      <c r="Q126">
-        <v>1</v>
-      </c>
-      <c r="R126" t="s">
-        <v>157</v>
-      </c>
-      <c r="S126" s="4">
-        <v>21.896999999999998</v>
-      </c>
-      <c r="T126" s="4">
-        <v>557.78399999999999</v>
-      </c>
-    </row>
-    <row r="127" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N127" t="s">
-        <v>155</v>
-      </c>
-      <c r="O127" s="2">
-        <v>42560</v>
-      </c>
-      <c r="P127" t="s">
-        <v>160</v>
-      </c>
-      <c r="Q127">
-        <v>2</v>
-      </c>
-      <c r="R127" t="s">
-        <v>157</v>
-      </c>
-      <c r="S127" s="4">
-        <v>20.867000000000001</v>
-      </c>
-      <c r="T127" s="4">
-        <v>601.40700000000004</v>
-      </c>
-    </row>
-    <row r="128" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N128" t="s">
-        <v>155</v>
-      </c>
-      <c r="O128" s="2">
-        <v>42560</v>
-      </c>
-      <c r="P128" t="s">
-        <v>160</v>
-      </c>
-      <c r="Q128">
-        <v>1</v>
-      </c>
-      <c r="R128" t="s">
-        <v>166</v>
-      </c>
-      <c r="S128" s="4">
-        <v>23.751000000000001</v>
-      </c>
-      <c r="T128" s="4">
-        <v>658.15599999999995</v>
-      </c>
-    </row>
-    <row r="129" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N129" t="s">
-        <v>155</v>
-      </c>
-      <c r="O129" s="2">
-        <v>42560</v>
-      </c>
-      <c r="P129" t="s">
-        <v>160</v>
-      </c>
-      <c r="Q129">
-        <v>2</v>
-      </c>
-      <c r="R129" t="s">
-        <v>166</v>
-      </c>
-      <c r="S129" s="4">
-        <v>26.366</v>
-      </c>
-      <c r="T129" s="4">
-        <v>698.62300000000005</v>
-      </c>
-    </row>
-    <row r="130" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N130" t="s">
-        <v>155</v>
-      </c>
-      <c r="O130" s="2">
-        <v>42560</v>
-      </c>
-      <c r="P130" t="s">
-        <v>164</v>
-      </c>
-      <c r="Q130">
-        <v>1</v>
-      </c>
-      <c r="R130" t="s">
-        <v>157</v>
-      </c>
-      <c r="S130" s="4">
-        <v>14.429</v>
-      </c>
-      <c r="T130" s="4">
-        <v>684.39800000000002</v>
-      </c>
-    </row>
-    <row r="131" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N131" t="s">
-        <v>155</v>
-      </c>
-      <c r="O131" s="2">
-        <v>42560</v>
-      </c>
-      <c r="P131" t="s">
-        <v>161</v>
-      </c>
-      <c r="Q131">
-        <v>2</v>
-      </c>
-      <c r="R131" t="s">
-        <v>157</v>
-      </c>
-      <c r="S131" s="4">
-        <v>13.281000000000001</v>
-      </c>
-      <c r="T131" s="4">
-        <v>656.971</v>
-      </c>
-    </row>
-    <row r="132" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N132" t="s">
-        <v>155</v>
-      </c>
-      <c r="O132" s="2">
-        <v>42560</v>
-      </c>
-      <c r="P132" t="s">
-        <v>161</v>
-      </c>
-      <c r="Q132">
-        <v>1</v>
-      </c>
-      <c r="R132" t="s">
-        <v>166</v>
-      </c>
-      <c r="S132" s="4">
-        <v>33.229999999999997</v>
-      </c>
-      <c r="T132" s="4">
-        <v>812.01400000000001</v>
-      </c>
-    </row>
-    <row r="133" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N133" t="s">
-        <v>155</v>
-      </c>
-      <c r="O133" s="2">
-        <v>42560</v>
-      </c>
-      <c r="P133" t="s">
-        <v>161</v>
-      </c>
-      <c r="Q133">
-        <v>2</v>
-      </c>
-      <c r="R133" t="s">
-        <v>166</v>
-      </c>
-      <c r="S133" s="4">
-        <v>27.706</v>
-      </c>
-      <c r="T133" s="4">
-        <v>733.98599999999999</v>
-      </c>
-    </row>
-    <row r="134" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N134" t="s">
-        <v>155</v>
-      </c>
-      <c r="O134" s="2">
-        <v>42560</v>
-      </c>
-      <c r="P134" t="s">
-        <v>162</v>
-      </c>
-      <c r="Q134">
-        <v>1</v>
-      </c>
-      <c r="R134" t="s">
-        <v>157</v>
-      </c>
-      <c r="S134" s="4">
-        <v>12.446999999999999</v>
-      </c>
-      <c r="T134" s="4">
-        <v>616.60900000000004</v>
-      </c>
-    </row>
-    <row r="135" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N135" t="s">
-        <v>155</v>
-      </c>
-      <c r="O135" s="2">
-        <v>42560</v>
-      </c>
-      <c r="P135" t="s">
-        <v>162</v>
-      </c>
-      <c r="Q135">
-        <v>2</v>
-      </c>
-      <c r="R135" t="s">
-        <v>157</v>
-      </c>
-      <c r="S135" s="4">
-        <v>12.634</v>
-      </c>
-      <c r="T135" s="4">
-        <v>647.70399999999995</v>
-      </c>
-    </row>
-    <row r="136" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N136" t="s">
-        <v>155</v>
-      </c>
-      <c r="O136" s="2">
-        <v>42560</v>
-      </c>
-      <c r="P136" t="s">
-        <v>162</v>
-      </c>
-      <c r="Q136">
-        <v>1</v>
-      </c>
-      <c r="R136" t="s">
-        <v>166</v>
-      </c>
-      <c r="S136" s="4">
-        <v>23.128</v>
-      </c>
-      <c r="T136" s="4">
-        <v>699.20899999999995</v>
-      </c>
-    </row>
-    <row r="137" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N137" t="s">
-        <v>155</v>
-      </c>
-      <c r="O137" s="2">
-        <v>42560</v>
-      </c>
-      <c r="P137" t="s">
-        <v>162</v>
-      </c>
-      <c r="Q137">
-        <v>2</v>
-      </c>
-      <c r="R137" t="s">
-        <v>166</v>
-      </c>
-      <c r="S137" s="4">
-        <v>25.699000000000002</v>
-      </c>
-      <c r="T137" s="4">
-        <v>685.72400000000005</v>
-      </c>
-    </row>
-    <row r="138" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N138" t="s">
-        <v>155</v>
-      </c>
-      <c r="O138" s="2">
-        <v>42560</v>
-      </c>
-      <c r="P138" t="s">
-        <v>163</v>
-      </c>
-      <c r="Q138">
-        <v>1</v>
-      </c>
-      <c r="R138" t="s">
-        <v>157</v>
-      </c>
-      <c r="S138" s="4">
-        <v>16.486000000000001</v>
-      </c>
-      <c r="T138" s="4">
-        <v>564.49400000000003</v>
-      </c>
-    </row>
-    <row r="139" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N139" t="s">
-        <v>155</v>
-      </c>
-      <c r="O139" s="2">
-        <v>42560</v>
-      </c>
-      <c r="P139" t="s">
-        <v>163</v>
-      </c>
-      <c r="Q139">
-        <v>2</v>
-      </c>
-      <c r="R139" t="s">
-        <v>157</v>
-      </c>
-      <c r="S139" s="4">
-        <v>15.699</v>
-      </c>
-      <c r="T139" s="4">
-        <v>570.13099999999997</v>
-      </c>
-    </row>
-    <row r="140" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N140" t="s">
-        <v>155</v>
-      </c>
-      <c r="O140" s="2">
-        <v>42560</v>
-      </c>
-      <c r="P140" t="s">
-        <v>163</v>
-      </c>
-      <c r="Q140">
-        <v>1</v>
-      </c>
-      <c r="R140" t="s">
-        <v>166</v>
-      </c>
-      <c r="S140" s="4">
-        <v>20.771000000000001</v>
-      </c>
-      <c r="T140" s="4">
-        <v>630.41999999999996</v>
-      </c>
-    </row>
-    <row r="141" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N141" t="s">
-        <v>155</v>
-      </c>
-      <c r="O141" s="2">
-        <v>42560</v>
-      </c>
-      <c r="P141" t="s">
-        <v>163</v>
-      </c>
-      <c r="Q141">
-        <v>2</v>
-      </c>
-      <c r="R141" t="s">
-        <v>166</v>
-      </c>
-      <c r="S141" s="4">
-        <v>21.384</v>
-      </c>
-      <c r="T141" s="4">
-        <v>717.84699999999998</v>
-      </c>
-    </row>
-    <row r="142" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N142" t="s">
-        <v>155</v>
-      </c>
-      <c r="O142" s="2">
-        <v>42561</v>
-      </c>
-      <c r="P142" t="s">
-        <v>164</v>
-      </c>
-      <c r="Q142">
-        <v>1</v>
-      </c>
-      <c r="R142" t="s">
-        <v>157</v>
-      </c>
-      <c r="S142" s="4">
-        <v>13.061999999999999</v>
-      </c>
-      <c r="T142" s="4">
-        <v>588.44500000000005</v>
-      </c>
-    </row>
-    <row r="143" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N143" t="s">
-        <v>155</v>
-      </c>
-      <c r="O143" s="2">
-        <v>42561</v>
-      </c>
-      <c r="P143" t="s">
-        <v>164</v>
-      </c>
-      <c r="Q143">
-        <v>2</v>
-      </c>
-      <c r="R143" t="s">
-        <v>157</v>
-      </c>
-      <c r="S143" s="4">
-        <v>13.428000000000001</v>
-      </c>
-      <c r="T143" s="4">
-        <v>571.63900000000001</v>
-      </c>
-    </row>
-    <row r="144" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N144" t="s">
-        <v>155</v>
-      </c>
-      <c r="O144" s="2">
-        <v>42561</v>
-      </c>
-      <c r="P144" t="s">
-        <v>164</v>
-      </c>
-      <c r="Q144">
-        <v>1</v>
-      </c>
-      <c r="R144" t="s">
-        <v>166</v>
-      </c>
-      <c r="S144" s="4">
-        <v>18.321000000000002</v>
-      </c>
-      <c r="T144" s="4">
-        <v>613.00699999999995</v>
-      </c>
-    </row>
-    <row r="145" spans="14:20" x14ac:dyDescent="0.25">
-      <c r="N145" t="s">
-        <v>155</v>
-      </c>
-      <c r="O145" s="2">
-        <v>42561</v>
-      </c>
-      <c r="P145" t="s">
-        <v>164</v>
-      </c>
-      <c r="Q145">
-        <v>2</v>
-      </c>
-      <c r="R145" t="s">
-        <v>166</v>
-      </c>
-      <c r="S145" s="4">
-        <v>18.163</v>
-      </c>
-      <c r="T145" s="4">
-        <v>636.55999999999995</v>
+      <c r="B33">
+        <v>728.42599999999993</v>
+      </c>
+      <c r="C33">
+        <v>30.602499999999999</v>
+      </c>
+      <c r="D33">
+        <v>592.91949999999997</v>
+      </c>
+      <c r="E33">
+        <v>14.3355</v>
       </c>
     </row>
   </sheetData>

</xml_diff>